<commit_message>
Merged PR 191: Add rendering of superscript characters
* Add rendering of superscript characters
* Prevent crash if you try to edit structure which has any nested molecules or functional groups in ChemDoodleWeb

Related work items: #436
</commit_message>
<xml_diff>
--- a/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
+++ b/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\vso\chem4word\Version3-1\src\Chemistry\Chem4Word.Model\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\vsts\Chem4Word\Version3-1\src\Chemistry\Chem4Word.Model2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084F13D2-2269-4A6B-8933-71D63103DC95}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodicTable" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PeriodicTable!$A$1:$M$125</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -1323,7 +1324,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1856,7 +1857,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1888,7 +1889,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2166,14 +2167,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD20"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8634,7 +8635,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M125"/>
+  <autoFilter ref="A1:M125" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="A2:Q131">
     <sortCondition ref="C2:C131"/>
     <sortCondition ref="A2:A131"/>

</xml_diff>

<commit_message>
Merged PR 225: Final attempt to get the new periodic table committed.
As far as I am concerned, the table part works fine.  There may be problems with the actual dialog itself, but that's another task.

Related work items: #127
</commit_message>
<xml_diff>
--- a/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
+++ b/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
@@ -1,29 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\vsts\Chem4Word\Version3-1\src\Chemistry\Chem4Word.Model2\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\source\repos\Version3-1a\src\Chemistry\Chem4Word.Model2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084F13D2-2269-4A6B-8933-71D63103DC95}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C602D-CF88-4F85-8656-4E7389742CD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="1800" windowWidth="24870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodicTable" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PeriodicTable!$A$1:$M$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PeriodicTable!$A$1:$M$122</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="422">
   <si>
     <t>Symbol</t>
   </si>
@@ -1285,40 +1293,10 @@
     <t>C# Property - Copy into PeriodicTable.cs</t>
   </si>
   <si>
-    <t>Uut</t>
-  </si>
-  <si>
-    <t>Ununtrium</t>
-  </si>
-  <si>
-    <t>Uuq</t>
-  </si>
-  <si>
-    <t>Ununquadium</t>
-  </si>
-  <si>
-    <t>Uup</t>
-  </si>
-  <si>
-    <t>Ununpentium</t>
-  </si>
-  <si>
-    <t>Uuh</t>
-  </si>
-  <si>
-    <t>Ununhexium</t>
-  </si>
-  <si>
-    <t>Uus</t>
-  </si>
-  <si>
-    <t>Ununseptium</t>
-  </si>
-  <si>
-    <t>Uuo</t>
-  </si>
-  <si>
-    <t>Ununoctium</t>
+    <t>pseudo</t>
+  </si>
+  <si>
+    <t>232|233|234|235|236|238</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1443,7 @@
       <name val="Helv"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1645,12 +1623,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1813,11 +1785,9 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2168,13 +2138,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q131"/>
+  <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,7 +2158,7 @@
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
@@ -2278,6 +2248,15 @@
       <c r="I2">
         <v>0</v>
       </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>420</v>
+      </c>
       <c r="Q2" t="str">
         <f t="shared" ref="Q2:Q17" si="0">CONCATENATE("public Element ", A2, " { get; private set; } // ",B2," - Atomic Number ", C2)</f>
         <v>public Element Du { get; private set; } // Dummy - Atomic Number 0</v>
@@ -2311,6 +2290,15 @@
       <c r="I3">
         <v>0</v>
       </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s">
+        <v>420</v>
+      </c>
       <c r="Q3" t="str">
         <f t="shared" si="0"/>
         <v>public Element M { get; private set; } // Metal - Atomic Number 0</v>
@@ -2344,6 +2332,15 @@
       <c r="I4">
         <v>0</v>
       </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>420</v>
+      </c>
       <c r="Q4" t="str">
         <f t="shared" si="0"/>
         <v>public Element R { get; private set; } // Residue - Atomic Number 0</v>
@@ -2377,6 +2374,15 @@
       <c r="I5">
         <v>0</v>
       </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>19</v>
+      </c>
+      <c r="P5" t="s">
+        <v>420</v>
+      </c>
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
         <v>public Element X { get; private set; } // Halogen - Atomic Number 0</v>
@@ -2410,6 +2416,15 @@
       <c r="I6">
         <v>2</v>
       </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>19</v>
+      </c>
+      <c r="P6" t="s">
+        <v>420</v>
+      </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
         <v>public Element D { get; private set; } // Deuterium - Atomic Number 1</v>
@@ -2497,6 +2512,15 @@
       <c r="I8">
         <v>3</v>
       </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>19</v>
+      </c>
+      <c r="P8" t="s">
+        <v>420</v>
+      </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
         <v>public Element T { get; private set; } // Tritium - Atomic Number 1</v>
@@ -7141,6 +7165,9 @@
       <c r="J99" s="1" t="s">
         <v>175</v>
       </c>
+      <c r="K99" s="1" t="s">
+        <v>421</v>
+      </c>
       <c r="L99">
         <v>3</v>
       </c>
@@ -7895,7 +7922,7 @@
         <v>406</v>
       </c>
       <c r="Q114" t="str">
-        <f t="shared" ref="Q114:Q131" si="4">CONCATENATE("public Element ", A114, " { get; private set; } // ",B114," - Atomic Number ", C114)</f>
+        <f t="shared" ref="Q114:Q125" si="4">CONCATENATE("public Element ", A114, " { get; private set; } // ",B114," - Atomic Number ", C114)</f>
         <v>public Element Bh { get; private set; } // Bohrium - Atomic Number 107</v>
       </c>
     </row>
@@ -8160,59 +8187,57 @@
         <v>public Element Nh { get; private set; } // Nihonium - Atomic Number 113</v>
       </c>
     </row>
-    <row r="121" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="C121" s="3">
-        <v>113</v>
-      </c>
-      <c r="D121" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E121" s="3" t="s">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>397</v>
+      </c>
+      <c r="B121" t="s">
+        <v>395</v>
+      </c>
+      <c r="C121">
+        <v>114</v>
+      </c>
+      <c r="D121" t="b">
+        <v>0</v>
+      </c>
+      <c r="E121" t="s">
         <v>379</v>
       </c>
-      <c r="F121" s="3">
-        <v>0</v>
-      </c>
-      <c r="G121" s="3">
-        <v>0</v>
-      </c>
-      <c r="H121" s="3">
-        <v>0</v>
-      </c>
-      <c r="I121" s="3">
-        <v>0</v>
-      </c>
-      <c r="J121" s="2"/>
-      <c r="K121" s="2"/>
-      <c r="N121" s="3">
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="N121">
         <v>6</v>
       </c>
-      <c r="O121" s="3">
-        <v>12</v>
-      </c>
-      <c r="P121" s="3" t="s">
+      <c r="O121">
+        <v>13</v>
+      </c>
+      <c r="P121" t="s">
         <v>409</v>
       </c>
-      <c r="Q121" s="3" t="str">
+      <c r="Q121" t="str">
         <f t="shared" si="4"/>
-        <v>public Element Uut { get; private set; } // Ununtrium - Atomic Number 113</v>
+        <v>public Element Fl { get; private set; } // Flerovium - Atomic Number 114</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="B122" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="C122">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D122" t="b">
         <v>0</v>
@@ -8236,69 +8261,67 @@
         <v>6</v>
       </c>
       <c r="O122">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P122" t="s">
         <v>409</v>
       </c>
       <c r="Q122" t="str">
         <f t="shared" si="4"/>
-        <v>public Element Fl { get; private set; } // Flerovium - Atomic Number 114</v>
-      </c>
-    </row>
-    <row r="123" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="C123" s="3">
-        <v>114</v>
-      </c>
-      <c r="D123" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E123" s="3" t="s">
+        <v>public Element Mc { get; private set; } // Moscovium - Atomic Number 115</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>398</v>
+      </c>
+      <c r="B123" t="s">
+        <v>396</v>
+      </c>
+      <c r="C123">
+        <v>116</v>
+      </c>
+      <c r="D123" t="b">
+        <v>0</v>
+      </c>
+      <c r="E123" t="s">
         <v>379</v>
       </c>
-      <c r="F123" s="3">
-        <v>0</v>
-      </c>
-      <c r="G123" s="3">
-        <v>0</v>
-      </c>
-      <c r="H123" s="3">
-        <v>0</v>
-      </c>
-      <c r="I123" s="3">
-        <v>0</v>
-      </c>
-      <c r="J123" s="2"/>
-      <c r="K123" s="2"/>
-      <c r="N123" s="3">
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="N123">
         <v>6</v>
       </c>
-      <c r="O123" s="3">
-        <v>13</v>
-      </c>
-      <c r="P123" s="3" t="s">
+      <c r="O123">
+        <v>15</v>
+      </c>
+      <c r="P123" t="s">
         <v>409</v>
       </c>
-      <c r="Q123" s="3" t="str">
+      <c r="Q123" t="str">
         <f t="shared" si="4"/>
-        <v>public Element Uuq { get; private set; } // Ununquadium - Atomic Number 114</v>
+        <v>public Element Lv { get; private set; } // Livermorium - Atomic Number 116</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B124" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C124">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D124" t="b">
         <v>0</v>
@@ -8322,323 +8345,63 @@
         <v>6</v>
       </c>
       <c r="O124">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P124" t="s">
         <v>409</v>
       </c>
       <c r="Q124" t="str">
         <f t="shared" si="4"/>
-        <v>public Element Mc { get; private set; } // Moscovium - Atomic Number 115</v>
-      </c>
-    </row>
-    <row r="125" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="C125" s="3">
-        <v>115</v>
-      </c>
-      <c r="D125" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E125" s="3" t="s">
+        <v>public Element Ts { get; private set; } // Tennessine - Atomic Number 117</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>413</v>
+      </c>
+      <c r="B125" t="s">
+        <v>417</v>
+      </c>
+      <c r="C125">
+        <v>118</v>
+      </c>
+      <c r="D125" t="b">
+        <v>0</v>
+      </c>
+      <c r="E125" t="s">
         <v>379</v>
       </c>
-      <c r="F125" s="3">
-        <v>0</v>
-      </c>
-      <c r="G125" s="3">
-        <v>0</v>
-      </c>
-      <c r="H125" s="3">
-        <v>0</v>
-      </c>
-      <c r="I125" s="3">
-        <v>0</v>
-      </c>
-      <c r="J125" s="2"/>
-      <c r="K125" s="2"/>
-      <c r="N125" s="3">
+      <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>0</v>
+      </c>
+      <c r="N125">
         <v>6</v>
       </c>
-      <c r="O125" s="3">
-        <v>14</v>
-      </c>
-      <c r="P125" s="3" t="s">
+      <c r="O125">
+        <v>17</v>
+      </c>
+      <c r="P125" t="s">
         <v>409</v>
       </c>
-      <c r="Q125" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>public Element Uup { get; private set; } // Ununpentium - Atomic Number 115</v>
-      </c>
-    </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>398</v>
-      </c>
-      <c r="B126" t="s">
-        <v>396</v>
-      </c>
-      <c r="C126">
-        <v>116</v>
-      </c>
-      <c r="D126" t="b">
-        <v>0</v>
-      </c>
-      <c r="E126" t="s">
-        <v>379</v>
-      </c>
-      <c r="F126">
-        <v>0</v>
-      </c>
-      <c r="G126">
-        <v>0</v>
-      </c>
-      <c r="H126">
-        <v>0</v>
-      </c>
-      <c r="I126">
-        <v>0</v>
-      </c>
-      <c r="N126">
-        <v>6</v>
-      </c>
-      <c r="O126">
-        <v>15</v>
-      </c>
-      <c r="P126" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q126" t="str">
-        <f t="shared" si="4"/>
-        <v>public Element Lv { get; private set; } // Livermorium - Atomic Number 116</v>
-      </c>
-    </row>
-    <row r="127" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="C127" s="3">
-        <v>116</v>
-      </c>
-      <c r="D127" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F127" s="3">
-        <v>0</v>
-      </c>
-      <c r="G127" s="3">
-        <v>0</v>
-      </c>
-      <c r="H127" s="3">
-        <v>0</v>
-      </c>
-      <c r="I127" s="3">
-        <v>0</v>
-      </c>
-      <c r="J127" s="2"/>
-      <c r="K127" s="2"/>
-      <c r="N127" s="3">
-        <v>6</v>
-      </c>
-      <c r="O127" s="3">
-        <v>15</v>
-      </c>
-      <c r="P127" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q127" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>public Element Uuh { get; private set; } // Ununhexium - Atomic Number 116</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>412</v>
-      </c>
-      <c r="B128" t="s">
-        <v>416</v>
-      </c>
-      <c r="C128">
-        <v>117</v>
-      </c>
-      <c r="D128" t="b">
-        <v>0</v>
-      </c>
-      <c r="E128" t="s">
-        <v>379</v>
-      </c>
-      <c r="F128">
-        <v>0</v>
-      </c>
-      <c r="G128">
-        <v>0</v>
-      </c>
-      <c r="H128">
-        <v>0</v>
-      </c>
-      <c r="I128">
-        <v>0</v>
-      </c>
-      <c r="N128">
-        <v>6</v>
-      </c>
-      <c r="O128">
-        <v>16</v>
-      </c>
-      <c r="P128" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q128" t="str">
-        <f t="shared" si="4"/>
-        <v>public Element Ts { get; private set; } // Tennessine - Atomic Number 117</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="C129" s="3">
-        <v>117</v>
-      </c>
-      <c r="D129" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F129" s="3">
-        <v>0</v>
-      </c>
-      <c r="G129" s="3">
-        <v>0</v>
-      </c>
-      <c r="H129" s="3">
-        <v>0</v>
-      </c>
-      <c r="I129" s="3">
-        <v>0</v>
-      </c>
-      <c r="J129" s="2"/>
-      <c r="K129" s="2"/>
-      <c r="N129" s="3">
-        <v>6</v>
-      </c>
-      <c r="O129" s="3">
-        <v>16</v>
-      </c>
-      <c r="P129" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q129" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>public Element Uus { get; private set; } // Ununseptium - Atomic Number 117</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>413</v>
-      </c>
-      <c r="B130" t="s">
-        <v>417</v>
-      </c>
-      <c r="C130">
-        <v>118</v>
-      </c>
-      <c r="D130" t="b">
-        <v>0</v>
-      </c>
-      <c r="E130" t="s">
-        <v>379</v>
-      </c>
-      <c r="F130">
-        <v>0</v>
-      </c>
-      <c r="G130">
-        <v>0</v>
-      </c>
-      <c r="H130">
-        <v>0</v>
-      </c>
-      <c r="I130">
-        <v>0</v>
-      </c>
-      <c r="N130">
-        <v>6</v>
-      </c>
-      <c r="O130">
-        <v>17</v>
-      </c>
-      <c r="P130" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q130" t="str">
+      <c r="Q125" t="str">
         <f t="shared" si="4"/>
         <v>public Element Og { get; private set; } // Oganesson - Atomic Number 118</v>
       </c>
     </row>
-    <row r="131" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="C131" s="3">
-        <v>118</v>
-      </c>
-      <c r="D131" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E131" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F131" s="3">
-        <v>0</v>
-      </c>
-      <c r="G131" s="3">
-        <v>0</v>
-      </c>
-      <c r="H131" s="3">
-        <v>0</v>
-      </c>
-      <c r="I131" s="3">
-        <v>0</v>
-      </c>
-      <c r="J131" s="2"/>
-      <c r="K131" s="2"/>
-      <c r="N131" s="3">
-        <v>6</v>
-      </c>
-      <c r="O131" s="3">
-        <v>17</v>
-      </c>
-      <c r="P131" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q131" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>public Element Uuo { get; private set; } // Ununoctium - Atomic Number 118</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:M125" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState ref="A2:Q131">
-    <sortCondition ref="C2:C131"/>
-    <sortCondition ref="A2:A131"/>
+  <autoFilter ref="A1:M122" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q125">
+    <sortCondition ref="C2:C125"/>
+    <sortCondition ref="A2:A125"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Merged PR 294: Dialogs all consistent in style
You *may* find them austere.  You *will* find them consistent.

Related work items: #619
</commit_message>
<xml_diff>
--- a/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
+++ b/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\source\repos\Version3-1a\src\Chemistry\Chem4Word.Model2\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\source\repos\Version3-1\src\Chemistry\Chem4Word.Model2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0C602D-CF88-4F85-8656-4E7389742CD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8160E8-E4C6-4D14-803D-69CC5C5DD6AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="1800" windowWidth="24870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodicTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="421">
   <si>
     <t>Symbol</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Carbon</t>
-  </si>
-  <si>
-    <t>#909090</t>
   </si>
   <si>
     <t>2|3|4</t>
@@ -2141,10 +2138,10 @@
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J101" sqref="J101"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,25 +2196,25 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="L1" t="s">
         <v>384</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>385</v>
       </c>
-      <c r="M1" t="s">
-        <v>386</v>
-      </c>
       <c r="N1" t="s">
+        <v>391</v>
+      </c>
+      <c r="O1" t="s">
         <v>392</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>393</v>
       </c>
-      <c r="P1" t="s">
-        <v>394</v>
-      </c>
       <c r="Q1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -2255,7 +2252,7 @@
         <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Q2" t="str">
         <f t="shared" ref="Q2:Q17" si="0">CONCATENATE("public Element ", A2, " { get; private set; } // ",B2," - Atomic Number ", C2)</f>
@@ -2297,7 +2294,7 @@
         <v>19</v>
       </c>
       <c r="P3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Q3" t="str">
         <f t="shared" si="0"/>
@@ -2339,7 +2336,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="0"/>
@@ -2381,7 +2378,7 @@
         <v>19</v>
       </c>
       <c r="P5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
@@ -2423,7 +2420,7 @@
         <v>19</v>
       </c>
       <c r="P6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
@@ -2462,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -2477,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="0"/>
@@ -2519,7 +2516,7 @@
         <v>19</v>
       </c>
       <c r="P8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
@@ -2558,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L9">
         <v>18</v>
@@ -2573,7 +2570,7 @@
         <v>17</v>
       </c>
       <c r="P9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="0"/>
@@ -2624,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="0"/>
@@ -2675,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q11" t="str">
         <f t="shared" si="0"/>
@@ -2714,7 +2711,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L12">
         <v>13</v>
@@ -2729,7 +2726,7 @@
         <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="0"/>
@@ -2750,7 +2747,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>378</v>
       </c>
       <c r="F13">
         <v>0.76</v>
@@ -2765,10 +2762,10 @@
         <v>12.010999999999999</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L13">
         <v>14</v>
@@ -2783,7 +2780,7 @@
         <v>13</v>
       </c>
       <c r="P13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="0"/>
@@ -2792,10 +2789,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
       </c>
       <c r="C14">
         <v>7</v>
@@ -2804,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14">
         <v>0.71</v>
@@ -2819,10 +2816,10 @@
         <v>14.006740000000001</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L14">
         <v>15</v>
@@ -2837,7 +2834,7 @@
         <v>14</v>
       </c>
       <c r="P14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="0"/>
@@ -2846,10 +2843,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
         <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
       </c>
       <c r="C15">
         <v>8</v>
@@ -2858,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15">
         <v>0.66</v>
@@ -2876,7 +2873,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L15">
         <v>16</v>
@@ -2891,7 +2888,7 @@
         <v>15</v>
       </c>
       <c r="P15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="0"/>
@@ -2900,10 +2897,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>49</v>
       </c>
       <c r="C16">
         <v>9</v>
@@ -2912,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16">
         <v>0.56999999999999995</v>
@@ -2945,7 +2942,7 @@
         <v>16</v>
       </c>
       <c r="P16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="0"/>
@@ -2954,10 +2951,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -2966,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17">
         <v>0.57999999999999996</v>
@@ -2996,7 +2993,7 @@
         <v>17</v>
       </c>
       <c r="P17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="0"/>
@@ -3005,10 +3002,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
         <v>54</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
       </c>
       <c r="C18">
         <v>11</v>
@@ -3017,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>1.66</v>
@@ -3047,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" ref="Q18:Q49" si="1">CONCATENATE("public Element ", A18, " { get; private set; } // ",B18," - Atomic Number ", C18)</f>
@@ -3056,10 +3053,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
         <v>57</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
       </c>
       <c r="C19">
         <v>12</v>
@@ -3068,7 +3065,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19">
         <v>1.41</v>
@@ -3098,7 +3095,7 @@
         <v>1</v>
       </c>
       <c r="P19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="1"/>
@@ -3107,10 +3104,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
         <v>60</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
       </c>
       <c r="C20">
         <v>13</v>
@@ -3119,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20">
         <v>1.21</v>
@@ -3149,7 +3146,7 @@
         <v>12</v>
       </c>
       <c r="P20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="1"/>
@@ -3158,10 +3155,10 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
         <v>63</v>
-      </c>
-      <c r="B21" t="s">
-        <v>64</v>
       </c>
       <c r="C21">
         <v>14</v>
@@ -3170,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21">
         <v>1.1100000000000001</v>
@@ -3200,7 +3197,7 @@
         <v>13</v>
       </c>
       <c r="P21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="1"/>
@@ -3209,10 +3206,10 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
         <v>66</v>
-      </c>
-      <c r="B22" t="s">
-        <v>67</v>
       </c>
       <c r="C22">
         <v>15</v>
@@ -3221,7 +3218,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22">
         <v>1.07</v>
@@ -3236,7 +3233,7 @@
         <v>30.973762000000001</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L22">
         <v>15</v>
@@ -3251,7 +3248,7 @@
         <v>14</v>
       </c>
       <c r="P22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="1"/>
@@ -3260,10 +3257,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
         <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -3272,7 +3269,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23">
         <v>1.05</v>
@@ -3287,7 +3284,7 @@
         <v>32.066000000000003</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L23">
         <v>16</v>
@@ -3302,7 +3299,7 @@
         <v>15</v>
       </c>
       <c r="P23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="1"/>
@@ -3311,10 +3308,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
         <v>73</v>
-      </c>
-      <c r="B24" t="s">
-        <v>74</v>
       </c>
       <c r="C24">
         <v>17</v>
@@ -3323,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F24">
         <v>1.02</v>
@@ -3338,10 +3335,10 @@
         <v>35.4527</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L24">
         <v>17</v>
@@ -3356,7 +3353,7 @@
         <v>16</v>
       </c>
       <c r="P24" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="1"/>
@@ -3365,10 +3362,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
         <v>77</v>
-      </c>
-      <c r="B25" t="s">
-        <v>78</v>
       </c>
       <c r="C25">
         <v>18</v>
@@ -3377,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25">
         <v>1.06</v>
@@ -3407,7 +3404,7 @@
         <v>17</v>
       </c>
       <c r="P25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="1"/>
@@ -3416,10 +3413,10 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
         <v>80</v>
-      </c>
-      <c r="B26" t="s">
-        <v>81</v>
       </c>
       <c r="C26">
         <v>19</v>
@@ -3428,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F26">
         <v>2.0299999999999998</v>
@@ -3458,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="1"/>
@@ -3467,10 +3464,10 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
         <v>83</v>
-      </c>
-      <c r="B27" t="s">
-        <v>84</v>
       </c>
       <c r="C27">
         <v>20</v>
@@ -3479,7 +3476,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F27">
         <v>1.76</v>
@@ -3509,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="P27" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="1"/>
@@ -3518,10 +3515,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
         <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>87</v>
       </c>
       <c r="C28">
         <v>21</v>
@@ -3530,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F28">
         <v>1.7</v>
@@ -3560,7 +3557,7 @@
         <v>2</v>
       </c>
       <c r="P28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="1"/>
@@ -3569,10 +3566,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" t="s">
         <v>89</v>
-      </c>
-      <c r="B29" t="s">
-        <v>90</v>
       </c>
       <c r="C29">
         <v>22</v>
@@ -3581,7 +3578,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F29">
         <v>1.6</v>
@@ -3596,7 +3593,7 @@
         <v>47.88</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L29">
         <v>4</v>
@@ -3611,7 +3608,7 @@
         <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q29" t="str">
         <f t="shared" si="1"/>
@@ -3620,10 +3617,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
         <v>92</v>
-      </c>
-      <c r="B30" t="s">
-        <v>93</v>
       </c>
       <c r="C30">
         <v>23</v>
@@ -3632,7 +3629,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F30">
         <v>1.53</v>
@@ -3647,7 +3644,7 @@
         <v>50.941499999999998</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L30">
         <v>5</v>
@@ -3662,7 +3659,7 @@
         <v>4</v>
       </c>
       <c r="P30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" si="1"/>
@@ -3671,10 +3668,10 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" t="s">
         <v>96</v>
-      </c>
-      <c r="B31" t="s">
-        <v>97</v>
       </c>
       <c r="C31">
         <v>24</v>
@@ -3683,7 +3680,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F31">
         <v>1.39</v>
@@ -3698,7 +3695,7 @@
         <v>51.996099999999998</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L31">
         <v>6</v>
@@ -3713,7 +3710,7 @@
         <v>5</v>
       </c>
       <c r="P31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" si="1"/>
@@ -3722,10 +3719,10 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
         <v>100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>101</v>
       </c>
       <c r="C32">
         <v>25</v>
@@ -3734,7 +3731,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F32">
         <v>1.39</v>
@@ -3749,7 +3746,7 @@
         <v>54.938049999999997</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L32">
         <v>7</v>
@@ -3764,7 +3761,7 @@
         <v>6</v>
       </c>
       <c r="P32" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" si="1"/>
@@ -3773,10 +3770,10 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
         <v>104</v>
-      </c>
-      <c r="B33" t="s">
-        <v>105</v>
       </c>
       <c r="C33">
         <v>26</v>
@@ -3785,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F33">
         <v>1.32</v>
@@ -3800,7 +3797,7 @@
         <v>55.847000000000001</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L33">
         <v>8</v>
@@ -3815,7 +3812,7 @@
         <v>7</v>
       </c>
       <c r="P33" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" si="1"/>
@@ -3824,10 +3821,10 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
         <v>108</v>
-      </c>
-      <c r="B34" t="s">
-        <v>109</v>
       </c>
       <c r="C34">
         <v>27</v>
@@ -3836,7 +3833,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F34">
         <v>1.26</v>
@@ -3851,7 +3848,7 @@
         <v>58.933199999999999</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L34">
         <v>9</v>
@@ -3866,7 +3863,7 @@
         <v>8</v>
       </c>
       <c r="P34" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" si="1"/>
@@ -3875,10 +3872,10 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s">
         <v>112</v>
-      </c>
-      <c r="B35" t="s">
-        <v>113</v>
       </c>
       <c r="C35">
         <v>28</v>
@@ -3887,7 +3884,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35">
         <v>1.24</v>
@@ -3902,7 +3899,7 @@
         <v>58.693399999999997</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L35">
         <v>10</v>
@@ -3917,7 +3914,7 @@
         <v>9</v>
       </c>
       <c r="P35" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" si="1"/>
@@ -3926,10 +3923,10 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
         <v>116</v>
-      </c>
-      <c r="B36" t="s">
-        <v>117</v>
       </c>
       <c r="C36">
         <v>29</v>
@@ -3938,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F36">
         <v>1.32</v>
@@ -3953,7 +3950,7 @@
         <v>63.545999999999999</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L36">
         <v>11</v>
@@ -3968,7 +3965,7 @@
         <v>10</v>
       </c>
       <c r="P36" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" si="1"/>
@@ -3977,10 +3974,10 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" t="s">
         <v>120</v>
-      </c>
-      <c r="B37" t="s">
-        <v>121</v>
       </c>
       <c r="C37">
         <v>30</v>
@@ -3989,7 +3986,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F37">
         <v>1.22</v>
@@ -4019,7 +4016,7 @@
         <v>11</v>
       </c>
       <c r="P37" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" si="1"/>
@@ -4028,10 +4025,10 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
         <v>123</v>
-      </c>
-      <c r="B38" t="s">
-        <v>124</v>
       </c>
       <c r="C38">
         <v>31</v>
@@ -4040,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F38">
         <v>1.22</v>
@@ -4055,7 +4052,7 @@
         <v>69.722999999999999</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L38">
         <v>13</v>
@@ -4070,7 +4067,7 @@
         <v>12</v>
       </c>
       <c r="P38" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" si="1"/>
@@ -4079,10 +4076,10 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" t="s">
         <v>126</v>
-      </c>
-      <c r="B39" t="s">
-        <v>127</v>
       </c>
       <c r="C39">
         <v>32</v>
@@ -4091,7 +4088,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F39">
         <v>1.2</v>
@@ -4106,7 +4103,7 @@
         <v>72.61</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L39">
         <v>14</v>
@@ -4121,7 +4118,7 @@
         <v>13</v>
       </c>
       <c r="P39" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" si="1"/>
@@ -4130,10 +4127,10 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>129</v>
+      </c>
+      <c r="B40" t="s">
         <v>130</v>
-      </c>
-      <c r="B40" t="s">
-        <v>131</v>
       </c>
       <c r="C40">
         <v>33</v>
@@ -4142,7 +4139,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F40">
         <v>1.19</v>
@@ -4157,7 +4154,7 @@
         <v>74.921589999999995</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L40">
         <v>15</v>
@@ -4172,7 +4169,7 @@
         <v>14</v>
       </c>
       <c r="P40" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" si="1"/>
@@ -4181,10 +4178,10 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" t="s">
         <v>134</v>
-      </c>
-      <c r="B41" t="s">
-        <v>135</v>
       </c>
       <c r="C41">
         <v>34</v>
@@ -4193,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F41">
         <v>1.2</v>
@@ -4208,7 +4205,7 @@
         <v>78.959999999999994</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L41">
         <v>16</v>
@@ -4223,7 +4220,7 @@
         <v>15</v>
       </c>
       <c r="P41" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" si="1"/>
@@ -4232,10 +4229,10 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" t="s">
         <v>138</v>
-      </c>
-      <c r="B42" t="s">
-        <v>139</v>
       </c>
       <c r="C42">
         <v>35</v>
@@ -4244,7 +4241,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F42">
         <v>1.2</v>
@@ -4259,7 +4256,7 @@
         <v>79.903999999999996</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L42">
         <v>17</v>
@@ -4274,7 +4271,7 @@
         <v>16</v>
       </c>
       <c r="P42" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" si="1"/>
@@ -4283,10 +4280,10 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" t="s">
         <v>141</v>
-      </c>
-      <c r="B43" t="s">
-        <v>142</v>
       </c>
       <c r="C43">
         <v>36</v>
@@ -4295,7 +4292,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F43">
         <v>1.1599999999999999</v>
@@ -4325,7 +4322,7 @@
         <v>17</v>
       </c>
       <c r="P43" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" si="1"/>
@@ -4334,10 +4331,10 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" t="s">
         <v>144</v>
-      </c>
-      <c r="B44" t="s">
-        <v>145</v>
       </c>
       <c r="C44">
         <v>37</v>
@@ -4346,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F44">
         <v>2.2000000000000002</v>
@@ -4361,7 +4358,7 @@
         <v>85.467799999999997</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L44">
         <v>1</v>
@@ -4376,7 +4373,7 @@
         <v>0</v>
       </c>
       <c r="P44" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" si="1"/>
@@ -4385,10 +4382,10 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>147</v>
+      </c>
+      <c r="B45" t="s">
         <v>148</v>
-      </c>
-      <c r="B45" t="s">
-        <v>149</v>
       </c>
       <c r="C45">
         <v>38</v>
@@ -4397,7 +4394,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F45">
         <v>1.95</v>
@@ -4427,7 +4424,7 @@
         <v>1</v>
       </c>
       <c r="P45" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" si="1"/>
@@ -4436,10 +4433,10 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" t="s">
         <v>151</v>
-      </c>
-      <c r="B46" t="s">
-        <v>152</v>
       </c>
       <c r="C46">
         <v>39</v>
@@ -4448,7 +4445,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F46">
         <v>1.9</v>
@@ -4478,7 +4475,7 @@
         <v>2</v>
       </c>
       <c r="P46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" si="1"/>
@@ -4487,10 +4484,10 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47" t="s">
         <v>154</v>
-      </c>
-      <c r="B47" t="s">
-        <v>155</v>
       </c>
       <c r="C47">
         <v>40</v>
@@ -4499,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F47">
         <v>1.75</v>
@@ -4514,7 +4511,7 @@
         <v>91.224000000000004</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L47">
         <v>4</v>
@@ -4529,7 +4526,7 @@
         <v>3</v>
       </c>
       <c r="P47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" si="1"/>
@@ -4538,10 +4535,10 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" t="s">
         <v>157</v>
-      </c>
-      <c r="B48" t="s">
-        <v>158</v>
       </c>
       <c r="C48">
         <v>41</v>
@@ -4550,7 +4547,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F48">
         <v>1.64</v>
@@ -4565,7 +4562,7 @@
         <v>92.906379999999999</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L48">
         <v>5</v>
@@ -4580,7 +4577,7 @@
         <v>4</v>
       </c>
       <c r="P48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" si="1"/>
@@ -4589,10 +4586,10 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49" t="s">
         <v>161</v>
-      </c>
-      <c r="B49" t="s">
-        <v>162</v>
       </c>
       <c r="C49">
         <v>42</v>
@@ -4601,7 +4598,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F49">
         <v>1.54</v>
@@ -4616,7 +4613,7 @@
         <v>95.94</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L49">
         <v>6</v>
@@ -4631,7 +4628,7 @@
         <v>5</v>
       </c>
       <c r="P49" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q49" t="str">
         <f t="shared" si="1"/>
@@ -4640,10 +4637,10 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>163</v>
+      </c>
+      <c r="B50" t="s">
         <v>164</v>
-      </c>
-      <c r="B50" t="s">
-        <v>165</v>
       </c>
       <c r="C50">
         <v>43</v>
@@ -4652,7 +4649,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F50">
         <v>1.47</v>
@@ -4667,7 +4664,7 @@
         <v>-97.907200000000003</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L50">
         <v>7</v>
@@ -4682,7 +4679,7 @@
         <v>6</v>
       </c>
       <c r="P50" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q50" t="str">
         <f t="shared" ref="Q50:Q81" si="2">CONCATENATE("public Element ", A50, " { get; private set; } // ",B50," - Atomic Number ", C50)</f>
@@ -4691,10 +4688,10 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" t="s">
         <v>168</v>
-      </c>
-      <c r="B51" t="s">
-        <v>169</v>
       </c>
       <c r="C51">
         <v>44</v>
@@ -4703,7 +4700,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F51">
         <v>1.46</v>
@@ -4718,7 +4715,7 @@
         <v>101.07</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L51">
         <v>8</v>
@@ -4733,7 +4730,7 @@
         <v>7</v>
       </c>
       <c r="P51" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q51" t="str">
         <f t="shared" si="2"/>
@@ -4742,10 +4739,10 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>171</v>
+      </c>
+      <c r="B52" t="s">
         <v>172</v>
-      </c>
-      <c r="B52" t="s">
-        <v>173</v>
       </c>
       <c r="C52">
         <v>45</v>
@@ -4754,7 +4751,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F52">
         <v>1.42</v>
@@ -4769,7 +4766,7 @@
         <v>102.9055</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L52">
         <v>9</v>
@@ -4784,7 +4781,7 @@
         <v>8</v>
       </c>
       <c r="P52" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q52" t="str">
         <f t="shared" si="2"/>
@@ -4793,10 +4790,10 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>175</v>
+      </c>
+      <c r="B53" t="s">
         <v>176</v>
-      </c>
-      <c r="B53" t="s">
-        <v>177</v>
       </c>
       <c r="C53">
         <v>46</v>
@@ -4805,7 +4802,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F53">
         <v>1.39</v>
@@ -4820,7 +4817,7 @@
         <v>106.42</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L53">
         <v>10</v>
@@ -4835,7 +4832,7 @@
         <v>9</v>
       </c>
       <c r="P53" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q53" t="str">
         <f t="shared" si="2"/>
@@ -4844,10 +4841,10 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" t="s">
         <v>179</v>
-      </c>
-      <c r="B54" t="s">
-        <v>180</v>
       </c>
       <c r="C54">
         <v>47</v>
@@ -4856,7 +4853,7 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F54">
         <v>1.45</v>
@@ -4871,7 +4868,7 @@
         <v>107.8682</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L54">
         <v>11</v>
@@ -4886,7 +4883,7 @@
         <v>10</v>
       </c>
       <c r="P54" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q54" t="str">
         <f t="shared" si="2"/>
@@ -4895,10 +4892,10 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" t="s">
         <v>182</v>
-      </c>
-      <c r="B55" t="s">
-        <v>183</v>
       </c>
       <c r="C55">
         <v>48</v>
@@ -4907,7 +4904,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F55">
         <v>1.44</v>
@@ -4937,7 +4934,7 @@
         <v>11</v>
       </c>
       <c r="P55" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q55" t="str">
         <f t="shared" si="2"/>
@@ -4946,10 +4943,10 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" t="s">
         <v>185</v>
-      </c>
-      <c r="B56" t="s">
-        <v>186</v>
       </c>
       <c r="C56">
         <v>49</v>
@@ -4958,7 +4955,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F56">
         <v>1.42</v>
@@ -4973,7 +4970,7 @@
         <v>114.818</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L56">
         <v>13</v>
@@ -4988,7 +4985,7 @@
         <v>12</v>
       </c>
       <c r="P56" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q56" t="str">
         <f t="shared" si="2"/>
@@ -4997,10 +4994,10 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>188</v>
+      </c>
+      <c r="B57" t="s">
         <v>189</v>
-      </c>
-      <c r="B57" t="s">
-        <v>190</v>
       </c>
       <c r="C57">
         <v>50</v>
@@ -5009,7 +5006,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F57">
         <v>1.39</v>
@@ -5024,7 +5021,7 @@
         <v>118.71</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L57">
         <v>14</v>
@@ -5039,7 +5036,7 @@
         <v>13</v>
       </c>
       <c r="P57" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q57" t="str">
         <f t="shared" si="2"/>
@@ -5048,10 +5045,10 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" t="s">
         <v>192</v>
-      </c>
-      <c r="B58" t="s">
-        <v>193</v>
       </c>
       <c r="C58">
         <v>51</v>
@@ -5060,7 +5057,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F58">
         <v>1.39</v>
@@ -5075,7 +5072,7 @@
         <v>121.75700000000001</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L58">
         <v>15</v>
@@ -5090,7 +5087,7 @@
         <v>14</v>
       </c>
       <c r="P58" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q58" t="str">
         <f t="shared" si="2"/>
@@ -5099,10 +5096,10 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" t="s">
         <v>196</v>
-      </c>
-      <c r="B59" t="s">
-        <v>197</v>
       </c>
       <c r="C59">
         <v>52</v>
@@ -5111,7 +5108,7 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F59">
         <v>1.38</v>
@@ -5126,7 +5123,7 @@
         <v>127.6</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L59">
         <v>16</v>
@@ -5141,7 +5138,7 @@
         <v>15</v>
       </c>
       <c r="P59" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q59" t="str">
         <f t="shared" si="2"/>
@@ -5150,10 +5147,10 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>198</v>
+      </c>
+      <c r="B60" t="s">
         <v>199</v>
-      </c>
-      <c r="B60" t="s">
-        <v>200</v>
       </c>
       <c r="C60">
         <v>53</v>
@@ -5162,7 +5159,7 @@
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F60">
         <v>1.39</v>
@@ -5177,7 +5174,7 @@
         <v>126.90447</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L60">
         <v>17</v>
@@ -5192,7 +5189,7 @@
         <v>16</v>
       </c>
       <c r="P60" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q60" t="str">
         <f t="shared" si="2"/>
@@ -5201,10 +5198,10 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" t="s">
         <v>202</v>
-      </c>
-      <c r="B61" t="s">
-        <v>203</v>
       </c>
       <c r="C61">
         <v>54</v>
@@ -5213,7 +5210,7 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F61">
         <v>1.4</v>
@@ -5243,7 +5240,7 @@
         <v>17</v>
       </c>
       <c r="P61" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q61" t="str">
         <f t="shared" si="2"/>
@@ -5252,10 +5249,10 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>204</v>
+      </c>
+      <c r="B62" t="s">
         <v>205</v>
-      </c>
-      <c r="B62" t="s">
-        <v>206</v>
       </c>
       <c r="C62">
         <v>55</v>
@@ -5264,7 +5261,7 @@
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F62">
         <v>2.44</v>
@@ -5294,7 +5291,7 @@
         <v>0</v>
       </c>
       <c r="P62" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q62" t="str">
         <f t="shared" si="2"/>
@@ -5303,10 +5300,10 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>207</v>
+      </c>
+      <c r="B63" t="s">
         <v>208</v>
-      </c>
-      <c r="B63" t="s">
-        <v>209</v>
       </c>
       <c r="C63">
         <v>56</v>
@@ -5315,7 +5312,7 @@
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F63">
         <v>2.15</v>
@@ -5345,7 +5342,7 @@
         <v>1</v>
       </c>
       <c r="P63" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q63" t="str">
         <f t="shared" si="2"/>
@@ -5354,10 +5351,10 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>210</v>
+      </c>
+      <c r="B64" t="s">
         <v>211</v>
-      </c>
-      <c r="B64" t="s">
-        <v>212</v>
       </c>
       <c r="C64">
         <v>57</v>
@@ -5366,7 +5363,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F64">
         <v>2.0699999999999998</v>
@@ -5396,7 +5393,7 @@
         <v>2</v>
       </c>
       <c r="P64" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q64" t="str">
         <f t="shared" si="2"/>
@@ -5405,10 +5402,10 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>213</v>
+      </c>
+      <c r="B65" t="s">
         <v>214</v>
-      </c>
-      <c r="B65" t="s">
-        <v>215</v>
       </c>
       <c r="C65">
         <v>58</v>
@@ -5417,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F65">
         <v>2.04</v>
@@ -5432,7 +5429,7 @@
         <v>140.11500000000001</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L65">
         <v>3</v>
@@ -5447,7 +5444,7 @@
         <v>3</v>
       </c>
       <c r="P65" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q65" t="str">
         <f t="shared" si="2"/>
@@ -5456,10 +5453,10 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>217</v>
+      </c>
+      <c r="B66" t="s">
         <v>218</v>
-      </c>
-      <c r="B66" t="s">
-        <v>219</v>
       </c>
       <c r="C66">
         <v>59</v>
@@ -5468,7 +5465,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F66">
         <v>2.0299999999999998</v>
@@ -5498,7 +5495,7 @@
         <v>4</v>
       </c>
       <c r="P66" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q66" t="str">
         <f t="shared" si="2"/>
@@ -5507,10 +5504,10 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>220</v>
+      </c>
+      <c r="B67" t="s">
         <v>221</v>
-      </c>
-      <c r="B67" t="s">
-        <v>222</v>
       </c>
       <c r="C67">
         <v>60</v>
@@ -5519,7 +5516,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F67">
         <v>2.0099999999999998</v>
@@ -5549,7 +5546,7 @@
         <v>5</v>
       </c>
       <c r="P67" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q67" t="str">
         <f t="shared" si="2"/>
@@ -5558,10 +5555,10 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>223</v>
+      </c>
+      <c r="B68" t="s">
         <v>224</v>
-      </c>
-      <c r="B68" t="s">
-        <v>225</v>
       </c>
       <c r="C68">
         <v>61</v>
@@ -5570,7 +5567,7 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F68">
         <v>1.99</v>
@@ -5600,7 +5597,7 @@
         <v>6</v>
       </c>
       <c r="P68" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q68" t="str">
         <f t="shared" si="2"/>
@@ -5609,10 +5606,10 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>226</v>
+      </c>
+      <c r="B69" t="s">
         <v>227</v>
-      </c>
-      <c r="B69" t="s">
-        <v>228</v>
       </c>
       <c r="C69">
         <v>62</v>
@@ -5621,7 +5618,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F69">
         <v>1.98</v>
@@ -5636,7 +5633,7 @@
         <v>150.36000000000001</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L69">
         <v>3</v>
@@ -5651,7 +5648,7 @@
         <v>7</v>
       </c>
       <c r="P69" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q69" t="str">
         <f t="shared" si="2"/>
@@ -5660,10 +5657,10 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>229</v>
+      </c>
+      <c r="B70" t="s">
         <v>230</v>
-      </c>
-      <c r="B70" t="s">
-        <v>231</v>
       </c>
       <c r="C70">
         <v>63</v>
@@ -5672,7 +5669,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F70">
         <v>1.98</v>
@@ -5687,7 +5684,7 @@
         <v>151.965</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L70">
         <v>3</v>
@@ -5702,7 +5699,7 @@
         <v>8</v>
       </c>
       <c r="P70" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q70" t="str">
         <f t="shared" si="2"/>
@@ -5711,10 +5708,10 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>232</v>
+      </c>
+      <c r="B71" t="s">
         <v>233</v>
-      </c>
-      <c r="B71" t="s">
-        <v>234</v>
       </c>
       <c r="C71">
         <v>64</v>
@@ -5723,7 +5720,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F71">
         <v>1.96</v>
@@ -5753,7 +5750,7 @@
         <v>9</v>
       </c>
       <c r="P71" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q71" t="str">
         <f t="shared" si="2"/>
@@ -5762,10 +5759,10 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>235</v>
+      </c>
+      <c r="B72" t="s">
         <v>236</v>
-      </c>
-      <c r="B72" t="s">
-        <v>237</v>
       </c>
       <c r="C72">
         <v>65</v>
@@ -5774,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F72">
         <v>1.94</v>
@@ -5789,7 +5786,7 @@
         <v>158.92534000000001</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L72">
         <v>3</v>
@@ -5804,7 +5801,7 @@
         <v>10</v>
       </c>
       <c r="P72" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q72" t="str">
         <f t="shared" si="2"/>
@@ -5813,10 +5810,10 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>238</v>
+      </c>
+      <c r="B73" t="s">
         <v>239</v>
-      </c>
-      <c r="B73" t="s">
-        <v>240</v>
       </c>
       <c r="C73">
         <v>66</v>
@@ -5825,7 +5822,7 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F73">
         <v>1.92</v>
@@ -5855,7 +5852,7 @@
         <v>11</v>
       </c>
       <c r="P73" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q73" t="str">
         <f t="shared" si="2"/>
@@ -5864,10 +5861,10 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>241</v>
+      </c>
+      <c r="B74" t="s">
         <v>242</v>
-      </c>
-      <c r="B74" t="s">
-        <v>243</v>
       </c>
       <c r="C74">
         <v>67</v>
@@ -5876,7 +5873,7 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F74">
         <v>1.92</v>
@@ -5906,7 +5903,7 @@
         <v>12</v>
       </c>
       <c r="P74" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q74" t="str">
         <f t="shared" si="2"/>
@@ -5915,10 +5912,10 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>244</v>
+      </c>
+      <c r="B75" t="s">
         <v>245</v>
-      </c>
-      <c r="B75" t="s">
-        <v>246</v>
       </c>
       <c r="C75">
         <v>68</v>
@@ -5927,7 +5924,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F75">
         <v>1.89</v>
@@ -5957,7 +5954,7 @@
         <v>13</v>
       </c>
       <c r="P75" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q75" t="str">
         <f t="shared" si="2"/>
@@ -5966,10 +5963,10 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>247</v>
+      </c>
+      <c r="B76" t="s">
         <v>248</v>
-      </c>
-      <c r="B76" t="s">
-        <v>249</v>
       </c>
       <c r="C76">
         <v>69</v>
@@ -5978,7 +5975,7 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F76">
         <v>1.9</v>
@@ -6008,7 +6005,7 @@
         <v>14</v>
       </c>
       <c r="P76" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q76" t="str">
         <f t="shared" si="2"/>
@@ -6017,10 +6014,10 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>250</v>
+      </c>
+      <c r="B77" t="s">
         <v>251</v>
-      </c>
-      <c r="B77" t="s">
-        <v>252</v>
       </c>
       <c r="C77">
         <v>70</v>
@@ -6029,7 +6026,7 @@
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F77">
         <v>1.87</v>
@@ -6044,7 +6041,7 @@
         <v>173.04</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L77">
         <v>3</v>
@@ -6059,7 +6056,7 @@
         <v>15</v>
       </c>
       <c r="P77" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q77" t="str">
         <f t="shared" si="2"/>
@@ -6068,10 +6065,10 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>253</v>
+      </c>
+      <c r="B78" t="s">
         <v>254</v>
-      </c>
-      <c r="B78" t="s">
-        <v>255</v>
       </c>
       <c r="C78">
         <v>71</v>
@@ -6080,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F78">
         <v>1.87</v>
@@ -6110,7 +6107,7 @@
         <v>2</v>
       </c>
       <c r="P78" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q78" t="str">
         <f t="shared" si="2"/>
@@ -6119,10 +6116,10 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>256</v>
+      </c>
+      <c r="B79" t="s">
         <v>257</v>
-      </c>
-      <c r="B79" t="s">
-        <v>258</v>
       </c>
       <c r="C79">
         <v>72</v>
@@ -6131,7 +6128,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F79">
         <v>1.75</v>
@@ -6161,7 +6158,7 @@
         <v>3</v>
       </c>
       <c r="P79" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q79" t="str">
         <f t="shared" si="2"/>
@@ -6170,10 +6167,10 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>259</v>
+      </c>
+      <c r="B80" t="s">
         <v>260</v>
-      </c>
-      <c r="B80" t="s">
-        <v>261</v>
       </c>
       <c r="C80">
         <v>73</v>
@@ -6182,7 +6179,7 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F80">
         <v>1.7</v>
@@ -6197,7 +6194,7 @@
         <v>180.9479</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L80">
         <v>5</v>
@@ -6212,7 +6209,7 @@
         <v>4</v>
       </c>
       <c r="P80" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q80" t="str">
         <f t="shared" si="2"/>
@@ -6221,10 +6218,10 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>262</v>
+      </c>
+      <c r="B81" t="s">
         <v>263</v>
-      </c>
-      <c r="B81" t="s">
-        <v>264</v>
       </c>
       <c r="C81">
         <v>74</v>
@@ -6233,7 +6230,7 @@
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F81">
         <v>1.62</v>
@@ -6248,7 +6245,7 @@
         <v>183.84</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L81">
         <v>6</v>
@@ -6263,7 +6260,7 @@
         <v>5</v>
       </c>
       <c r="P81" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q81" t="str">
         <f t="shared" si="2"/>
@@ -6272,10 +6269,10 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>265</v>
+      </c>
+      <c r="B82" t="s">
         <v>266</v>
-      </c>
-      <c r="B82" t="s">
-        <v>267</v>
       </c>
       <c r="C82">
         <v>75</v>
@@ -6284,7 +6281,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F82">
         <v>1.51</v>
@@ -6299,7 +6296,7 @@
         <v>186.20699999999999</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L82">
         <v>7</v>
@@ -6314,7 +6311,7 @@
         <v>6</v>
       </c>
       <c r="P82" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q82" t="str">
         <f t="shared" ref="Q82:Q113" si="3">CONCATENATE("public Element ", A82, " { get; private set; } // ",B82," - Atomic Number ", C82)</f>
@@ -6323,10 +6320,10 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>269</v>
+      </c>
+      <c r="B83" t="s">
         <v>270</v>
-      </c>
-      <c r="B83" t="s">
-        <v>271</v>
       </c>
       <c r="C83">
         <v>76</v>
@@ -6335,7 +6332,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F83">
         <v>1.44</v>
@@ -6350,7 +6347,7 @@
         <v>190.23</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L83">
         <v>8</v>
@@ -6365,7 +6362,7 @@
         <v>7</v>
       </c>
       <c r="P83" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q83" t="str">
         <f t="shared" si="3"/>
@@ -6374,10 +6371,10 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>273</v>
+      </c>
+      <c r="B84" t="s">
         <v>274</v>
-      </c>
-      <c r="B84" t="s">
-        <v>275</v>
       </c>
       <c r="C84">
         <v>77</v>
@@ -6386,7 +6383,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F84">
         <v>1.41</v>
@@ -6416,7 +6413,7 @@
         <v>8</v>
       </c>
       <c r="P84" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q84" t="str">
         <f t="shared" si="3"/>
@@ -6425,10 +6422,10 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>276</v>
+      </c>
+      <c r="B85" t="s">
         <v>277</v>
-      </c>
-      <c r="B85" t="s">
-        <v>278</v>
       </c>
       <c r="C85">
         <v>78</v>
@@ -6437,7 +6434,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F85">
         <v>1.36</v>
@@ -6452,7 +6449,7 @@
         <v>195.08</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L85">
         <v>10</v>
@@ -6467,7 +6464,7 @@
         <v>9</v>
       </c>
       <c r="P85" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q85" t="str">
         <f t="shared" si="3"/>
@@ -6476,10 +6473,10 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>279</v>
+      </c>
+      <c r="B86" t="s">
         <v>280</v>
-      </c>
-      <c r="B86" t="s">
-        <v>281</v>
       </c>
       <c r="C86">
         <v>79</v>
@@ -6488,7 +6485,7 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F86">
         <v>1.36</v>
@@ -6503,7 +6500,7 @@
         <v>196.96654000000001</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L86">
         <v>11</v>
@@ -6518,7 +6515,7 @@
         <v>10</v>
       </c>
       <c r="P86" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q86" t="str">
         <f t="shared" si="3"/>
@@ -6527,10 +6524,10 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>283</v>
+      </c>
+      <c r="B87" t="s">
         <v>284</v>
-      </c>
-      <c r="B87" t="s">
-        <v>285</v>
       </c>
       <c r="C87">
         <v>80</v>
@@ -6539,7 +6536,7 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F87">
         <v>1.32</v>
@@ -6554,7 +6551,7 @@
         <v>200.59</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L87">
         <v>12</v>
@@ -6569,7 +6566,7 @@
         <v>11</v>
       </c>
       <c r="P87" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q87" t="str">
         <f t="shared" si="3"/>
@@ -6578,10 +6575,10 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>286</v>
+      </c>
+      <c r="B88" t="s">
         <v>287</v>
-      </c>
-      <c r="B88" t="s">
-        <v>288</v>
       </c>
       <c r="C88">
         <v>81</v>
@@ -6590,7 +6587,7 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F88">
         <v>1.45</v>
@@ -6605,7 +6602,7 @@
         <v>204.38329999999999</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L88">
         <v>13</v>
@@ -6620,7 +6617,7 @@
         <v>12</v>
       </c>
       <c r="P88" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q88" t="str">
         <f t="shared" si="3"/>
@@ -6629,10 +6626,10 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>289</v>
+      </c>
+      <c r="B89" t="s">
         <v>290</v>
-      </c>
-      <c r="B89" t="s">
-        <v>291</v>
       </c>
       <c r="C89">
         <v>82</v>
@@ -6641,7 +6638,7 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F89">
         <v>1.46</v>
@@ -6656,7 +6653,7 @@
         <v>207.2</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L89">
         <v>14</v>
@@ -6671,7 +6668,7 @@
         <v>13</v>
       </c>
       <c r="P89" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q89" t="str">
         <f t="shared" si="3"/>
@@ -6680,10 +6677,10 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>292</v>
+      </c>
+      <c r="B90" t="s">
         <v>293</v>
-      </c>
-      <c r="B90" t="s">
-        <v>294</v>
       </c>
       <c r="C90">
         <v>83</v>
@@ -6692,7 +6689,7 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F90">
         <v>1.48</v>
@@ -6707,7 +6704,7 @@
         <v>208.98036999999999</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L90">
         <v>15</v>
@@ -6722,7 +6719,7 @@
         <v>14</v>
       </c>
       <c r="P90" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q90" t="str">
         <f t="shared" si="3"/>
@@ -6731,10 +6728,10 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>295</v>
+      </c>
+      <c r="B91" t="s">
         <v>296</v>
-      </c>
-      <c r="B91" t="s">
-        <v>297</v>
       </c>
       <c r="C91">
         <v>84</v>
@@ -6743,7 +6740,7 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F91">
         <v>1.4</v>
@@ -6758,7 +6755,7 @@
         <v>-208.98240000000001</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L91">
         <v>16</v>
@@ -6773,7 +6770,7 @@
         <v>15</v>
       </c>
       <c r="P91" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q91" t="str">
         <f t="shared" si="3"/>
@@ -6782,10 +6779,10 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>299</v>
+      </c>
+      <c r="B92" t="s">
         <v>300</v>
-      </c>
-      <c r="B92" t="s">
-        <v>301</v>
       </c>
       <c r="C92">
         <v>85</v>
@@ -6794,7 +6791,7 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F92">
         <v>1.5</v>
@@ -6809,7 +6806,7 @@
         <v>-209.9871</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L92">
         <v>17</v>
@@ -6824,7 +6821,7 @@
         <v>16</v>
       </c>
       <c r="P92" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q92" t="str">
         <f t="shared" si="3"/>
@@ -6833,10 +6830,10 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>302</v>
+      </c>
+      <c r="B93" t="s">
         <v>303</v>
-      </c>
-      <c r="B93" t="s">
-        <v>304</v>
       </c>
       <c r="C93">
         <v>86</v>
@@ -6845,7 +6842,7 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F93">
         <v>1.5</v>
@@ -6875,7 +6872,7 @@
         <v>17</v>
       </c>
       <c r="P93" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q93" t="str">
         <f t="shared" si="3"/>
@@ -6884,10 +6881,10 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>305</v>
+      </c>
+      <c r="B94" t="s">
         <v>306</v>
-      </c>
-      <c r="B94" t="s">
-        <v>307</v>
       </c>
       <c r="C94">
         <v>87</v>
@@ -6896,7 +6893,7 @@
         <v>0</v>
       </c>
       <c r="E94" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F94">
         <v>2.6</v>
@@ -6926,7 +6923,7 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q94" t="str">
         <f t="shared" si="3"/>
@@ -6935,10 +6932,10 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>308</v>
+      </c>
+      <c r="B95" t="s">
         <v>309</v>
-      </c>
-      <c r="B95" t="s">
-        <v>310</v>
       </c>
       <c r="C95">
         <v>88</v>
@@ -6947,7 +6944,7 @@
         <v>0</v>
       </c>
       <c r="E95" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F95">
         <v>2.21</v>
@@ -6977,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="P95" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q95" t="str">
         <f t="shared" si="3"/>
@@ -6986,10 +6983,10 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>311</v>
+      </c>
+      <c r="B96" t="s">
         <v>312</v>
-      </c>
-      <c r="B96" t="s">
-        <v>313</v>
       </c>
       <c r="C96">
         <v>89</v>
@@ -6998,7 +6995,7 @@
         <v>0</v>
       </c>
       <c r="E96" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F96">
         <v>2.15</v>
@@ -7025,7 +7022,7 @@
         <v>2</v>
       </c>
       <c r="P96" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q96" t="str">
         <f t="shared" si="3"/>
@@ -7034,10 +7031,10 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>314</v>
+      </c>
+      <c r="B97" t="s">
         <v>315</v>
-      </c>
-      <c r="B97" t="s">
-        <v>316</v>
       </c>
       <c r="C97">
         <v>90</v>
@@ -7046,7 +7043,7 @@
         <v>0</v>
       </c>
       <c r="E97" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F97">
         <v>2.06</v>
@@ -7076,7 +7073,7 @@
         <v>3</v>
       </c>
       <c r="P97" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q97" t="str">
         <f t="shared" si="3"/>
@@ -7085,10 +7082,10 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>317</v>
+      </c>
+      <c r="B98" t="s">
         <v>318</v>
-      </c>
-      <c r="B98" t="s">
-        <v>319</v>
       </c>
       <c r="C98">
         <v>91</v>
@@ -7097,7 +7094,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F98">
         <v>2</v>
@@ -7112,7 +7109,7 @@
         <v>231.03587999999999</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L98">
         <v>3</v>
@@ -7127,7 +7124,7 @@
         <v>4</v>
       </c>
       <c r="P98" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q98" t="str">
         <f t="shared" si="3"/>
@@ -7136,10 +7133,10 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>321</v>
+      </c>
+      <c r="B99" t="s">
         <v>322</v>
-      </c>
-      <c r="B99" t="s">
-        <v>323</v>
       </c>
       <c r="C99">
         <v>92</v>
@@ -7148,7 +7145,7 @@
         <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F99">
         <v>1.96</v>
@@ -7163,10 +7160,10 @@
         <v>238.02889999999999</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L99">
         <v>3</v>
@@ -7181,7 +7178,7 @@
         <v>5</v>
       </c>
       <c r="P99" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q99" t="str">
         <f t="shared" si="3"/>
@@ -7190,10 +7187,10 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>324</v>
+      </c>
+      <c r="B100" t="s">
         <v>325</v>
-      </c>
-      <c r="B100" t="s">
-        <v>326</v>
       </c>
       <c r="C100">
         <v>93</v>
@@ -7202,7 +7199,7 @@
         <v>0</v>
       </c>
       <c r="E100" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F100">
         <v>1.9</v>
@@ -7217,7 +7214,7 @@
         <v>-237.04820000000001</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L100">
         <v>3</v>
@@ -7232,7 +7229,7 @@
         <v>6</v>
       </c>
       <c r="P100" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q100" t="str">
         <f t="shared" si="3"/>
@@ -7241,10 +7238,10 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>328</v>
+      </c>
+      <c r="B101" t="s">
         <v>329</v>
-      </c>
-      <c r="B101" t="s">
-        <v>330</v>
       </c>
       <c r="C101">
         <v>94</v>
@@ -7253,7 +7250,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F101">
         <v>1.87</v>
@@ -7268,7 +7265,7 @@
         <v>-244.0642</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L101">
         <v>3</v>
@@ -7283,7 +7280,7 @@
         <v>7</v>
       </c>
       <c r="P101" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q101" t="str">
         <f t="shared" si="3"/>
@@ -7292,10 +7289,10 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>331</v>
+      </c>
+      <c r="B102" t="s">
         <v>332</v>
-      </c>
-      <c r="B102" t="s">
-        <v>333</v>
       </c>
       <c r="C102">
         <v>95</v>
@@ -7304,7 +7301,7 @@
         <v>0</v>
       </c>
       <c r="E102" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F102">
         <v>1.8</v>
@@ -7319,7 +7316,7 @@
         <v>-243.06139999999999</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L102">
         <v>3</v>
@@ -7334,7 +7331,7 @@
         <v>8</v>
       </c>
       <c r="P102" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q102" t="str">
         <f t="shared" si="3"/>
@@ -7343,10 +7340,10 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>334</v>
+      </c>
+      <c r="B103" t="s">
         <v>335</v>
-      </c>
-      <c r="B103" t="s">
-        <v>336</v>
       </c>
       <c r="C103">
         <v>96</v>
@@ -7355,7 +7352,7 @@
         <v>0</v>
       </c>
       <c r="E103" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F103">
         <v>1.69</v>
@@ -7370,7 +7367,7 @@
         <v>-247.0703</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L103">
         <v>3</v>
@@ -7385,7 +7382,7 @@
         <v>9</v>
       </c>
       <c r="P103" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q103" t="str">
         <f t="shared" si="3"/>
@@ -7394,10 +7391,10 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>337</v>
+      </c>
+      <c r="B104" t="s">
         <v>338</v>
-      </c>
-      <c r="B104" t="s">
-        <v>339</v>
       </c>
       <c r="C104">
         <v>97</v>
@@ -7406,7 +7403,7 @@
         <v>0</v>
       </c>
       <c r="E104" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -7421,7 +7418,7 @@
         <v>-247.0703</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L104">
         <v>3</v>
@@ -7436,7 +7433,7 @@
         <v>10</v>
       </c>
       <c r="P104" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q104" t="str">
         <f t="shared" si="3"/>
@@ -7445,10 +7442,10 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>340</v>
+      </c>
+      <c r="B105" t="s">
         <v>341</v>
-      </c>
-      <c r="B105" t="s">
-        <v>342</v>
       </c>
       <c r="C105">
         <v>98</v>
@@ -7457,7 +7454,7 @@
         <v>0</v>
       </c>
       <c r="E105" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -7484,7 +7481,7 @@
         <v>11</v>
       </c>
       <c r="P105" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q105" t="str">
         <f t="shared" si="3"/>
@@ -7493,10 +7490,10 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>343</v>
+      </c>
+      <c r="B106" t="s">
         <v>344</v>
-      </c>
-      <c r="B106" t="s">
-        <v>345</v>
       </c>
       <c r="C106">
         <v>99</v>
@@ -7505,7 +7502,7 @@
         <v>0</v>
       </c>
       <c r="E106" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F106">
         <v>0</v>
@@ -7532,7 +7529,7 @@
         <v>12</v>
       </c>
       <c r="P106" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q106" t="str">
         <f t="shared" si="3"/>
@@ -7541,10 +7538,10 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>346</v>
+      </c>
+      <c r="B107" t="s">
         <v>347</v>
-      </c>
-      <c r="B107" t="s">
-        <v>348</v>
       </c>
       <c r="C107">
         <v>100</v>
@@ -7553,7 +7550,7 @@
         <v>0</v>
       </c>
       <c r="E107" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F107">
         <v>0</v>
@@ -7580,7 +7577,7 @@
         <v>13</v>
       </c>
       <c r="P107" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q107" t="str">
         <f t="shared" si="3"/>
@@ -7589,10 +7586,10 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>349</v>
+      </c>
+      <c r="B108" t="s">
         <v>350</v>
-      </c>
-      <c r="B108" t="s">
-        <v>351</v>
       </c>
       <c r="C108">
         <v>101</v>
@@ -7601,7 +7598,7 @@
         <v>0</v>
       </c>
       <c r="E108" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F108">
         <v>0</v>
@@ -7616,7 +7613,7 @@
         <v>-258.09840000000003</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L108">
         <v>3</v>
@@ -7631,7 +7628,7 @@
         <v>14</v>
       </c>
       <c r="P108" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q108" t="str">
         <f t="shared" si="3"/>
@@ -7640,10 +7637,10 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>352</v>
+      </c>
+      <c r="B109" t="s">
         <v>353</v>
-      </c>
-      <c r="B109" t="s">
-        <v>354</v>
       </c>
       <c r="C109">
         <v>102</v>
@@ -7652,7 +7649,7 @@
         <v>0</v>
       </c>
       <c r="E109" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -7679,7 +7676,7 @@
         <v>15</v>
       </c>
       <c r="P109" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q109" t="str">
         <f t="shared" si="3"/>
@@ -7688,10 +7685,10 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>355</v>
+      </c>
+      <c r="B110" t="s">
         <v>356</v>
-      </c>
-      <c r="B110" t="s">
-        <v>357</v>
       </c>
       <c r="C110">
         <v>103</v>
@@ -7700,7 +7697,7 @@
         <v>0</v>
       </c>
       <c r="E110" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -7730,7 +7727,7 @@
         <v>2</v>
       </c>
       <c r="P110" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q110" t="str">
         <f t="shared" si="3"/>
@@ -7739,10 +7736,10 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>358</v>
+      </c>
+      <c r="B111" t="s">
         <v>359</v>
-      </c>
-      <c r="B111" t="s">
-        <v>360</v>
       </c>
       <c r="C111">
         <v>104</v>
@@ -7751,7 +7748,7 @@
         <v>0</v>
       </c>
       <c r="E111" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -7778,7 +7775,7 @@
         <v>3</v>
       </c>
       <c r="P111" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q111" t="str">
         <f t="shared" si="3"/>
@@ -7787,10 +7784,10 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>361</v>
+      </c>
+      <c r="B112" t="s">
         <v>362</v>
-      </c>
-      <c r="B112" t="s">
-        <v>363</v>
       </c>
       <c r="C112">
         <v>105</v>
@@ -7799,7 +7796,7 @@
         <v>0</v>
       </c>
       <c r="E112" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -7826,7 +7823,7 @@
         <v>4</v>
       </c>
       <c r="P112" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q112" t="str">
         <f t="shared" si="3"/>
@@ -7835,10 +7832,10 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>364</v>
+      </c>
+      <c r="B113" t="s">
         <v>365</v>
-      </c>
-      <c r="B113" t="s">
-        <v>366</v>
       </c>
       <c r="C113">
         <v>106</v>
@@ -7847,7 +7844,7 @@
         <v>0</v>
       </c>
       <c r="E113" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F113">
         <v>0</v>
@@ -7874,7 +7871,7 @@
         <v>5</v>
       </c>
       <c r="P113" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q113" t="str">
         <f t="shared" si="3"/>
@@ -7883,10 +7880,10 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>367</v>
+      </c>
+      <c r="B114" t="s">
         <v>368</v>
-      </c>
-      <c r="B114" t="s">
-        <v>369</v>
       </c>
       <c r="C114">
         <v>107</v>
@@ -7895,7 +7892,7 @@
         <v>0</v>
       </c>
       <c r="E114" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -7919,7 +7916,7 @@
         <v>6</v>
       </c>
       <c r="P114" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q114" t="str">
         <f t="shared" ref="Q114:Q125" si="4">CONCATENATE("public Element ", A114, " { get; private set; } // ",B114," - Atomic Number ", C114)</f>
@@ -7928,10 +7925,10 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>370</v>
+      </c>
+      <c r="B115" t="s">
         <v>371</v>
-      </c>
-      <c r="B115" t="s">
-        <v>372</v>
       </c>
       <c r="C115">
         <v>108</v>
@@ -7940,7 +7937,7 @@
         <v>0</v>
       </c>
       <c r="E115" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -7964,7 +7961,7 @@
         <v>7</v>
       </c>
       <c r="P115" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q115" t="str">
         <f t="shared" si="4"/>
@@ -7973,10 +7970,10 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>373</v>
+      </c>
+      <c r="B116" t="s">
         <v>374</v>
-      </c>
-      <c r="B116" t="s">
-        <v>375</v>
       </c>
       <c r="C116">
         <v>109</v>
@@ -7985,7 +7982,7 @@
         <v>0</v>
       </c>
       <c r="E116" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -8009,7 +8006,7 @@
         <v>8</v>
       </c>
       <c r="P116" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q116" t="str">
         <f t="shared" si="4"/>
@@ -8018,10 +8015,10 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>376</v>
+      </c>
+      <c r="B117" t="s">
         <v>377</v>
-      </c>
-      <c r="B117" t="s">
-        <v>378</v>
       </c>
       <c r="C117">
         <v>110</v>
@@ -8030,7 +8027,7 @@
         <v>0</v>
       </c>
       <c r="E117" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F117">
         <v>0</v>
@@ -8054,7 +8051,7 @@
         <v>9</v>
       </c>
       <c r="P117" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q117" t="str">
         <f t="shared" si="4"/>
@@ -8063,10 +8060,10 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>379</v>
+      </c>
+      <c r="B118" t="s">
         <v>380</v>
-      </c>
-      <c r="B118" t="s">
-        <v>381</v>
       </c>
       <c r="C118">
         <v>111</v>
@@ -8075,7 +8072,7 @@
         <v>0</v>
       </c>
       <c r="E118" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -8096,7 +8093,7 @@
         <v>10</v>
       </c>
       <c r="P118" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q118" t="str">
         <f t="shared" si="4"/>
@@ -8105,10 +8102,10 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>381</v>
+      </c>
+      <c r="B119" t="s">
         <v>382</v>
-      </c>
-      <c r="B119" t="s">
-        <v>383</v>
       </c>
       <c r="C119">
         <v>112</v>
@@ -8117,7 +8114,7 @@
         <v>0</v>
       </c>
       <c r="E119" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -8138,7 +8135,7 @@
         <v>11</v>
       </c>
       <c r="P119" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q119" t="str">
         <f t="shared" si="4"/>
@@ -8147,10 +8144,10 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B120" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C120">
         <v>113</v>
@@ -8159,7 +8156,7 @@
         <v>0</v>
       </c>
       <c r="E120" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F120">
         <v>0</v>
@@ -8180,7 +8177,7 @@
         <v>12</v>
       </c>
       <c r="P120" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q120" t="str">
         <f t="shared" si="4"/>
@@ -8189,10 +8186,10 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B121" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C121">
         <v>114</v>
@@ -8201,7 +8198,7 @@
         <v>0</v>
       </c>
       <c r="E121" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F121">
         <v>0</v>
@@ -8222,7 +8219,7 @@
         <v>13</v>
       </c>
       <c r="P121" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q121" t="str">
         <f t="shared" si="4"/>
@@ -8231,10 +8228,10 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B122" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C122">
         <v>115</v>
@@ -8243,7 +8240,7 @@
         <v>0</v>
       </c>
       <c r="E122" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F122">
         <v>0</v>
@@ -8264,7 +8261,7 @@
         <v>14</v>
       </c>
       <c r="P122" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q122" t="str">
         <f t="shared" si="4"/>
@@ -8273,10 +8270,10 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B123" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C123">
         <v>116</v>
@@ -8285,7 +8282,7 @@
         <v>0</v>
       </c>
       <c r="E123" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F123">
         <v>0</v>
@@ -8306,7 +8303,7 @@
         <v>15</v>
       </c>
       <c r="P123" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q123" t="str">
         <f t="shared" si="4"/>
@@ -8315,10 +8312,10 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B124" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C124">
         <v>117</v>
@@ -8327,7 +8324,7 @@
         <v>0</v>
       </c>
       <c r="E124" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F124">
         <v>0</v>
@@ -8348,7 +8345,7 @@
         <v>16</v>
       </c>
       <c r="P124" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q124" t="str">
         <f t="shared" si="4"/>
@@ -8357,10 +8354,10 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B125" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C125">
         <v>118</v>
@@ -8369,7 +8366,7 @@
         <v>0</v>
       </c>
       <c r="E125" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F125">
         <v>0</v>
@@ -8390,7 +8387,7 @@
         <v>17</v>
       </c>
       <c r="P125" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q125" t="str">
         <f t="shared" si="4"/>
@@ -8398,7 +8395,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M122" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M122" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M125">
+      <sortCondition ref="C1:C122"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q125">
     <sortCondition ref="C2:C125"/>
     <sortCondition ref="A2:A125"/>

</xml_diff>

<commit_message>
Merged PR 307: Stage 1 of preparation for beta release
- Stage 1 of preparation for beta release
- Change definition of FG to remove dictionary
- Allow coloured FG default to TP.Carbon if not set
- Allow default of Black for Atoms defined in PT

Related work items: #645
</commit_message>
<xml_diff>
--- a/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
+++ b/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\source\repos\Version3-1\src\Chemistry\Chem4Word.Model2\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8160E8-E4C6-4D14-803D-69CC5C5DD6AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodicTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="420">
   <si>
     <t>Symbol</t>
   </si>
@@ -1165,9 +1159,6 @@
   </si>
   <si>
     <t>Darmstadtium</t>
-  </si>
-  <si>
-    <t>#000000</t>
   </si>
   <si>
     <t>Rg</t>
@@ -1299,7 +1290,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1824,7 +1815,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 2" xfId="42"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1856,7 +1847,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2127,21 +2118,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,25 +2187,25 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="L1" t="s">
         <v>383</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>384</v>
       </c>
-      <c r="M1" t="s">
-        <v>385</v>
-      </c>
       <c r="N1" t="s">
+        <v>390</v>
+      </c>
+      <c r="O1" t="s">
         <v>391</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>392</v>
       </c>
-      <c r="P1" t="s">
-        <v>393</v>
-      </c>
       <c r="Q1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -2252,7 +2243,7 @@
         <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q2" t="str">
         <f t="shared" ref="Q2:Q17" si="0">CONCATENATE("public Element ", A2, " { get; private set; } // ",B2," - Atomic Number ", C2)</f>
@@ -2294,7 +2285,7 @@
         <v>19</v>
       </c>
       <c r="P3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q3" t="str">
         <f t="shared" si="0"/>
@@ -2336,7 +2327,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="0"/>
@@ -2378,7 +2369,7 @@
         <v>19</v>
       </c>
       <c r="P5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q5" t="str">
         <f t="shared" si="0"/>
@@ -2420,7 +2411,7 @@
         <v>19</v>
       </c>
       <c r="P6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q6" t="str">
         <f t="shared" si="0"/>
@@ -2474,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="0"/>
@@ -2516,7 +2507,7 @@
         <v>19</v>
       </c>
       <c r="P8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="0"/>
@@ -2570,7 +2561,7 @@
         <v>17</v>
       </c>
       <c r="P9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="0"/>
@@ -2621,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q10" t="str">
         <f t="shared" si="0"/>
@@ -2672,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q11" t="str">
         <f t="shared" si="0"/>
@@ -2711,7 +2702,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L12">
         <v>13</v>
@@ -2726,7 +2717,7 @@
         <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="0"/>
@@ -2746,9 +2737,6 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
-        <v>378</v>
-      </c>
       <c r="F13">
         <v>0.76</v>
       </c>
@@ -2762,10 +2750,10 @@
         <v>12.010999999999999</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L13">
         <v>14</v>
@@ -2780,7 +2768,7 @@
         <v>13</v>
       </c>
       <c r="P13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="0"/>
@@ -2819,7 +2807,7 @@
         <v>43</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L14">
         <v>15</v>
@@ -2834,7 +2822,7 @@
         <v>14</v>
       </c>
       <c r="P14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="0"/>
@@ -2873,7 +2861,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L15">
         <v>16</v>
@@ -2888,7 +2876,7 @@
         <v>15</v>
       </c>
       <c r="P15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="0"/>
@@ -2942,7 +2930,7 @@
         <v>16</v>
       </c>
       <c r="P16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="0"/>
@@ -2993,7 +2981,7 @@
         <v>17</v>
       </c>
       <c r="P17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="0"/>
@@ -3044,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" ref="Q18:Q49" si="1">CONCATENATE("public Element ", A18, " { get; private set; } // ",B18," - Atomic Number ", C18)</f>
@@ -3095,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="P19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="1"/>
@@ -3146,7 +3134,7 @@
         <v>12</v>
       </c>
       <c r="P20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="1"/>
@@ -3197,7 +3185,7 @@
         <v>13</v>
       </c>
       <c r="P21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="1"/>
@@ -3248,7 +3236,7 @@
         <v>14</v>
       </c>
       <c r="P22" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="1"/>
@@ -3299,7 +3287,7 @@
         <v>15</v>
       </c>
       <c r="P23" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="1"/>
@@ -3338,7 +3326,7 @@
         <v>75</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L24">
         <v>17</v>
@@ -3353,7 +3341,7 @@
         <v>16</v>
       </c>
       <c r="P24" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="1"/>
@@ -3404,7 +3392,7 @@
         <v>17</v>
       </c>
       <c r="P25" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="1"/>
@@ -3455,7 +3443,7 @@
         <v>0</v>
       </c>
       <c r="P26" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="1"/>
@@ -3506,7 +3494,7 @@
         <v>1</v>
       </c>
       <c r="P27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="1"/>
@@ -3557,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="P28" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="1"/>
@@ -3608,7 +3596,7 @@
         <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q29" t="str">
         <f t="shared" si="1"/>
@@ -3659,7 +3647,7 @@
         <v>4</v>
       </c>
       <c r="P30" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" si="1"/>
@@ -3710,7 +3698,7 @@
         <v>5</v>
       </c>
       <c r="P31" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" si="1"/>
@@ -3761,7 +3749,7 @@
         <v>6</v>
       </c>
       <c r="P32" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" si="1"/>
@@ -3812,7 +3800,7 @@
         <v>7</v>
       </c>
       <c r="P33" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" si="1"/>
@@ -3863,7 +3851,7 @@
         <v>8</v>
       </c>
       <c r="P34" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" si="1"/>
@@ -3914,7 +3902,7 @@
         <v>9</v>
       </c>
       <c r="P35" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" si="1"/>
@@ -3965,7 +3953,7 @@
         <v>10</v>
       </c>
       <c r="P36" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" si="1"/>
@@ -4016,7 +4004,7 @@
         <v>11</v>
       </c>
       <c r="P37" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" si="1"/>
@@ -4067,7 +4055,7 @@
         <v>12</v>
       </c>
       <c r="P38" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" si="1"/>
@@ -4118,7 +4106,7 @@
         <v>13</v>
       </c>
       <c r="P39" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" si="1"/>
@@ -4169,7 +4157,7 @@
         <v>14</v>
       </c>
       <c r="P40" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" si="1"/>
@@ -4220,7 +4208,7 @@
         <v>15</v>
       </c>
       <c r="P41" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" si="1"/>
@@ -4271,7 +4259,7 @@
         <v>16</v>
       </c>
       <c r="P42" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" si="1"/>
@@ -4322,7 +4310,7 @@
         <v>17</v>
       </c>
       <c r="P43" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" si="1"/>
@@ -4373,7 +4361,7 @@
         <v>0</v>
       </c>
       <c r="P44" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" si="1"/>
@@ -4424,7 +4412,7 @@
         <v>1</v>
       </c>
       <c r="P45" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" si="1"/>
@@ -4475,7 +4463,7 @@
         <v>2</v>
       </c>
       <c r="P46" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" si="1"/>
@@ -4526,7 +4514,7 @@
         <v>3</v>
       </c>
       <c r="P47" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" si="1"/>
@@ -4577,7 +4565,7 @@
         <v>4</v>
       </c>
       <c r="P48" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" si="1"/>
@@ -4628,7 +4616,7 @@
         <v>5</v>
       </c>
       <c r="P49" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q49" t="str">
         <f t="shared" si="1"/>
@@ -4679,7 +4667,7 @@
         <v>6</v>
       </c>
       <c r="P50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q50" t="str">
         <f t="shared" ref="Q50:Q81" si="2">CONCATENATE("public Element ", A50, " { get; private set; } // ",B50," - Atomic Number ", C50)</f>
@@ -4730,7 +4718,7 @@
         <v>7</v>
       </c>
       <c r="P51" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q51" t="str">
         <f t="shared" si="2"/>
@@ -4781,7 +4769,7 @@
         <v>8</v>
       </c>
       <c r="P52" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q52" t="str">
         <f t="shared" si="2"/>
@@ -4832,7 +4820,7 @@
         <v>9</v>
       </c>
       <c r="P53" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q53" t="str">
         <f t="shared" si="2"/>
@@ -4883,7 +4871,7 @@
         <v>10</v>
       </c>
       <c r="P54" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q54" t="str">
         <f t="shared" si="2"/>
@@ -4934,7 +4922,7 @@
         <v>11</v>
       </c>
       <c r="P55" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q55" t="str">
         <f t="shared" si="2"/>
@@ -4985,7 +4973,7 @@
         <v>12</v>
       </c>
       <c r="P56" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q56" t="str">
         <f t="shared" si="2"/>
@@ -5036,7 +5024,7 @@
         <v>13</v>
       </c>
       <c r="P57" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q57" t="str">
         <f t="shared" si="2"/>
@@ -5087,7 +5075,7 @@
         <v>14</v>
       </c>
       <c r="P58" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q58" t="str">
         <f t="shared" si="2"/>
@@ -5138,7 +5126,7 @@
         <v>15</v>
       </c>
       <c r="P59" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q59" t="str">
         <f t="shared" si="2"/>
@@ -5189,7 +5177,7 @@
         <v>16</v>
       </c>
       <c r="P60" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q60" t="str">
         <f t="shared" si="2"/>
@@ -5240,7 +5228,7 @@
         <v>17</v>
       </c>
       <c r="P61" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q61" t="str">
         <f t="shared" si="2"/>
@@ -5291,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="P62" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q62" t="str">
         <f t="shared" si="2"/>
@@ -5342,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="P63" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q63" t="str">
         <f t="shared" si="2"/>
@@ -5393,7 +5381,7 @@
         <v>2</v>
       </c>
       <c r="P64" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q64" t="str">
         <f t="shared" si="2"/>
@@ -5444,7 +5432,7 @@
         <v>3</v>
       </c>
       <c r="P65" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q65" t="str">
         <f t="shared" si="2"/>
@@ -5495,7 +5483,7 @@
         <v>4</v>
       </c>
       <c r="P66" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q66" t="str">
         <f t="shared" si="2"/>
@@ -5546,7 +5534,7 @@
         <v>5</v>
       </c>
       <c r="P67" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q67" t="str">
         <f t="shared" si="2"/>
@@ -5597,7 +5585,7 @@
         <v>6</v>
       </c>
       <c r="P68" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q68" t="str">
         <f t="shared" si="2"/>
@@ -5648,7 +5636,7 @@
         <v>7</v>
       </c>
       <c r="P69" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q69" t="str">
         <f t="shared" si="2"/>
@@ -5699,7 +5687,7 @@
         <v>8</v>
       </c>
       <c r="P70" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q70" t="str">
         <f t="shared" si="2"/>
@@ -5750,7 +5738,7 @@
         <v>9</v>
       </c>
       <c r="P71" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q71" t="str">
         <f t="shared" si="2"/>
@@ -5801,7 +5789,7 @@
         <v>10</v>
       </c>
       <c r="P72" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q72" t="str">
         <f t="shared" si="2"/>
@@ -5852,7 +5840,7 @@
         <v>11</v>
       </c>
       <c r="P73" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q73" t="str">
         <f t="shared" si="2"/>
@@ -5903,7 +5891,7 @@
         <v>12</v>
       </c>
       <c r="P74" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q74" t="str">
         <f t="shared" si="2"/>
@@ -5954,7 +5942,7 @@
         <v>13</v>
       </c>
       <c r="P75" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q75" t="str">
         <f t="shared" si="2"/>
@@ -6005,7 +5993,7 @@
         <v>14</v>
       </c>
       <c r="P76" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q76" t="str">
         <f t="shared" si="2"/>
@@ -6056,7 +6044,7 @@
         <v>15</v>
       </c>
       <c r="P77" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q77" t="str">
         <f t="shared" si="2"/>
@@ -6107,7 +6095,7 @@
         <v>2</v>
       </c>
       <c r="P78" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q78" t="str">
         <f t="shared" si="2"/>
@@ -6158,7 +6146,7 @@
         <v>3</v>
       </c>
       <c r="P79" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q79" t="str">
         <f t="shared" si="2"/>
@@ -6209,7 +6197,7 @@
         <v>4</v>
       </c>
       <c r="P80" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q80" t="str">
         <f t="shared" si="2"/>
@@ -6260,7 +6248,7 @@
         <v>5</v>
       </c>
       <c r="P81" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q81" t="str">
         <f t="shared" si="2"/>
@@ -6311,7 +6299,7 @@
         <v>6</v>
       </c>
       <c r="P82" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q82" t="str">
         <f t="shared" ref="Q82:Q113" si="3">CONCATENATE("public Element ", A82, " { get; private set; } // ",B82," - Atomic Number ", C82)</f>
@@ -6362,7 +6350,7 @@
         <v>7</v>
       </c>
       <c r="P83" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q83" t="str">
         <f t="shared" si="3"/>
@@ -6413,7 +6401,7 @@
         <v>8</v>
       </c>
       <c r="P84" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q84" t="str">
         <f t="shared" si="3"/>
@@ -6464,7 +6452,7 @@
         <v>9</v>
       </c>
       <c r="P85" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q85" t="str">
         <f t="shared" si="3"/>
@@ -6515,7 +6503,7 @@
         <v>10</v>
       </c>
       <c r="P86" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q86" t="str">
         <f t="shared" si="3"/>
@@ -6566,7 +6554,7 @@
         <v>11</v>
       </c>
       <c r="P87" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q87" t="str">
         <f t="shared" si="3"/>
@@ -6617,7 +6605,7 @@
         <v>12</v>
       </c>
       <c r="P88" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q88" t="str">
         <f t="shared" si="3"/>
@@ -6668,7 +6656,7 @@
         <v>13</v>
       </c>
       <c r="P89" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q89" t="str">
         <f t="shared" si="3"/>
@@ -6719,7 +6707,7 @@
         <v>14</v>
       </c>
       <c r="P90" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Q90" t="str">
         <f t="shared" si="3"/>
@@ -6770,7 +6758,7 @@
         <v>15</v>
       </c>
       <c r="P91" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q91" t="str">
         <f t="shared" si="3"/>
@@ -6821,7 +6809,7 @@
         <v>16</v>
       </c>
       <c r="P92" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q92" t="str">
         <f t="shared" si="3"/>
@@ -6872,7 +6860,7 @@
         <v>17</v>
       </c>
       <c r="P93" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="Q93" t="str">
         <f t="shared" si="3"/>
@@ -6923,7 +6911,7 @@
         <v>0</v>
       </c>
       <c r="P94" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q94" t="str">
         <f t="shared" si="3"/>
@@ -6974,7 +6962,7 @@
         <v>1</v>
       </c>
       <c r="P95" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q95" t="str">
         <f t="shared" si="3"/>
@@ -7022,7 +7010,7 @@
         <v>2</v>
       </c>
       <c r="P96" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q96" t="str">
         <f t="shared" si="3"/>
@@ -7073,7 +7061,7 @@
         <v>3</v>
       </c>
       <c r="P97" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q97" t="str">
         <f t="shared" si="3"/>
@@ -7124,7 +7112,7 @@
         <v>4</v>
       </c>
       <c r="P98" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q98" t="str">
         <f t="shared" si="3"/>
@@ -7163,7 +7151,7 @@
         <v>174</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L99">
         <v>3</v>
@@ -7178,7 +7166,7 @@
         <v>5</v>
       </c>
       <c r="P99" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q99" t="str">
         <f t="shared" si="3"/>
@@ -7229,7 +7217,7 @@
         <v>6</v>
       </c>
       <c r="P100" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q100" t="str">
         <f t="shared" si="3"/>
@@ -7280,7 +7268,7 @@
         <v>7</v>
       </c>
       <c r="P101" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q101" t="str">
         <f t="shared" si="3"/>
@@ -7331,7 +7319,7 @@
         <v>8</v>
       </c>
       <c r="P102" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q102" t="str">
         <f t="shared" si="3"/>
@@ -7382,7 +7370,7 @@
         <v>9</v>
       </c>
       <c r="P103" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q103" t="str">
         <f t="shared" si="3"/>
@@ -7433,7 +7421,7 @@
         <v>10</v>
       </c>
       <c r="P104" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q104" t="str">
         <f t="shared" si="3"/>
@@ -7481,7 +7469,7 @@
         <v>11</v>
       </c>
       <c r="P105" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q105" t="str">
         <f t="shared" si="3"/>
@@ -7529,7 +7517,7 @@
         <v>12</v>
       </c>
       <c r="P106" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q106" t="str">
         <f t="shared" si="3"/>
@@ -7577,7 +7565,7 @@
         <v>13</v>
       </c>
       <c r="P107" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q107" t="str">
         <f t="shared" si="3"/>
@@ -7628,7 +7616,7 @@
         <v>14</v>
       </c>
       <c r="P108" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q108" t="str">
         <f t="shared" si="3"/>
@@ -7676,7 +7664,7 @@
         <v>15</v>
       </c>
       <c r="P109" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q109" t="str">
         <f t="shared" si="3"/>
@@ -7727,7 +7715,7 @@
         <v>2</v>
       </c>
       <c r="P110" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q110" t="str">
         <f t="shared" si="3"/>
@@ -7775,7 +7763,7 @@
         <v>3</v>
       </c>
       <c r="P111" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q111" t="str">
         <f t="shared" si="3"/>
@@ -7823,7 +7811,7 @@
         <v>4</v>
       </c>
       <c r="P112" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q112" t="str">
         <f t="shared" si="3"/>
@@ -7871,7 +7859,7 @@
         <v>5</v>
       </c>
       <c r="P113" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q113" t="str">
         <f t="shared" si="3"/>
@@ -7916,7 +7904,7 @@
         <v>6</v>
       </c>
       <c r="P114" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q114" t="str">
         <f t="shared" ref="Q114:Q125" si="4">CONCATENATE("public Element ", A114, " { get; private set; } // ",B114," - Atomic Number ", C114)</f>
@@ -7961,7 +7949,7 @@
         <v>7</v>
       </c>
       <c r="P115" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q115" t="str">
         <f t="shared" si="4"/>
@@ -8006,7 +7994,7 @@
         <v>8</v>
       </c>
       <c r="P116" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q116" t="str">
         <f t="shared" si="4"/>
@@ -8026,9 +8014,6 @@
       <c r="D117" t="b">
         <v>0</v>
       </c>
-      <c r="E117" t="s">
-        <v>378</v>
-      </c>
       <c r="F117">
         <v>0</v>
       </c>
@@ -8051,7 +8036,7 @@
         <v>9</v>
       </c>
       <c r="P117" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q117" t="str">
         <f t="shared" si="4"/>
@@ -8060,10 +8045,10 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>378</v>
+      </c>
+      <c r="B118" t="s">
         <v>379</v>
-      </c>
-      <c r="B118" t="s">
-        <v>380</v>
       </c>
       <c r="C118">
         <v>111</v>
@@ -8071,9 +8056,6 @@
       <c r="D118" t="b">
         <v>0</v>
       </c>
-      <c r="E118" t="s">
-        <v>378</v>
-      </c>
       <c r="F118">
         <v>0</v>
       </c>
@@ -8093,7 +8075,7 @@
         <v>10</v>
       </c>
       <c r="P118" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q118" t="str">
         <f t="shared" si="4"/>
@@ -8102,10 +8084,10 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>380</v>
+      </c>
+      <c r="B119" t="s">
         <v>381</v>
-      </c>
-      <c r="B119" t="s">
-        <v>382</v>
       </c>
       <c r="C119">
         <v>112</v>
@@ -8113,9 +8095,6 @@
       <c r="D119" t="b">
         <v>0</v>
       </c>
-      <c r="E119" t="s">
-        <v>378</v>
-      </c>
       <c r="F119">
         <v>0</v>
       </c>
@@ -8135,7 +8114,7 @@
         <v>11</v>
       </c>
       <c r="P119" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Q119" t="str">
         <f t="shared" si="4"/>
@@ -8144,10 +8123,10 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B120" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C120">
         <v>113</v>
@@ -8155,9 +8134,6 @@
       <c r="D120" t="b">
         <v>0</v>
       </c>
-      <c r="E120" t="s">
-        <v>378</v>
-      </c>
       <c r="F120">
         <v>0</v>
       </c>
@@ -8177,7 +8153,7 @@
         <v>12</v>
       </c>
       <c r="P120" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q120" t="str">
         <f t="shared" si="4"/>
@@ -8186,10 +8162,10 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B121" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C121">
         <v>114</v>
@@ -8197,9 +8173,6 @@
       <c r="D121" t="b">
         <v>0</v>
       </c>
-      <c r="E121" t="s">
-        <v>378</v>
-      </c>
       <c r="F121">
         <v>0</v>
       </c>
@@ -8219,7 +8192,7 @@
         <v>13</v>
       </c>
       <c r="P121" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q121" t="str">
         <f t="shared" si="4"/>
@@ -8228,10 +8201,10 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B122" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C122">
         <v>115</v>
@@ -8239,9 +8212,6 @@
       <c r="D122" t="b">
         <v>0</v>
       </c>
-      <c r="E122" t="s">
-        <v>378</v>
-      </c>
       <c r="F122">
         <v>0</v>
       </c>
@@ -8261,7 +8231,7 @@
         <v>14</v>
       </c>
       <c r="P122" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q122" t="str">
         <f t="shared" si="4"/>
@@ -8270,10 +8240,10 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B123" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C123">
         <v>116</v>
@@ -8281,9 +8251,6 @@
       <c r="D123" t="b">
         <v>0</v>
       </c>
-      <c r="E123" t="s">
-        <v>378</v>
-      </c>
       <c r="F123">
         <v>0</v>
       </c>
@@ -8303,7 +8270,7 @@
         <v>15</v>
       </c>
       <c r="P123" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q123" t="str">
         <f t="shared" si="4"/>
@@ -8312,10 +8279,10 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B124" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C124">
         <v>117</v>
@@ -8323,9 +8290,6 @@
       <c r="D124" t="b">
         <v>0</v>
       </c>
-      <c r="E124" t="s">
-        <v>378</v>
-      </c>
       <c r="F124">
         <v>0</v>
       </c>
@@ -8345,7 +8309,7 @@
         <v>16</v>
       </c>
       <c r="P124" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q124" t="str">
         <f t="shared" si="4"/>
@@ -8354,10 +8318,10 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B125" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C125">
         <v>118</v>
@@ -8365,9 +8329,6 @@
       <c r="D125" t="b">
         <v>0</v>
       </c>
-      <c r="E125" t="s">
-        <v>378</v>
-      </c>
       <c r="F125">
         <v>0</v>
       </c>
@@ -8387,7 +8348,7 @@
         <v>17</v>
       </c>
       <c r="P125" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q125" t="str">
         <f t="shared" si="4"/>
@@ -8395,12 +8356,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M122" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M125">
+  <autoFilter ref="A1:M122">
+    <sortState ref="A2:M125">
       <sortCondition ref="C1:C122"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q125">
+  <sortState ref="A2:Q125">
     <sortCondition ref="C2:C125"/>
     <sortCondition ref="A2:A125"/>
   </sortState>

</xml_diff>

<commit_message>
Merged PR 331: Vesion 3.1.5 Beta 5
* Fix Unable to add a bond to R atom https://github.com/Chem4Word/Version3-1/issues/20
* Add ability to rotate bond to specific values https://github.com/Chem4Word/Version3-1/issues/10
* Bond length incorrect for new drawings https://github.com/Chem4Word/Version3-1/issues/27
* Fix placement of Functional Groups https://github.com/Chem4Word/Version3-1/issues/29
* Fix deleting of bonds connected to explicitly hidden C atoms causing invisible C atoms
* Remove c4w:Explicit on lone (Carbon) atoms on import, to prevent them from being invisible
* Performance improvements
* Fix doubling up of 2019 in Office detection

Related work items: #665, #683, #689, #692, #693, #694, #695
</commit_message>
<xml_diff>
--- a/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
+++ b/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\source\repos\Version3-1\src\Chemistry\Chem4Word.Model2\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE8FD7B-C9BB-45A3-8518-99E6548D1B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="1815" yWindow="1290" windowWidth="24870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodicTable" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="422">
   <si>
     <t>Symbol</t>
   </si>
@@ -1285,12 +1293,18 @@
   </si>
   <si>
     <t>232|233|234|235|236|238</t>
+  </si>
+  <si>
+    <t>0|1|2|3|4|5|6|7|8|9|10</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1815,7 +1829,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1847,7 +1861,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2118,21 +2132,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B105" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E123" sqref="E123"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,7 +2159,7 @@
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="29.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
@@ -2236,6 +2250,9 @@
       <c r="I2">
         <v>0</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N2">
         <v>0</v>
       </c>
@@ -2278,6 +2295,9 @@
       <c r="I3">
         <v>0</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N3">
         <v>1</v>
       </c>
@@ -2320,6 +2340,9 @@
       <c r="I4">
         <v>0</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N4">
         <v>2</v>
       </c>
@@ -2362,6 +2385,9 @@
       <c r="I5">
         <v>0</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N5">
         <v>3</v>
       </c>
@@ -2404,6 +2430,9 @@
       <c r="I6">
         <v>2</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>421</v>
+      </c>
       <c r="N6">
         <v>4</v>
       </c>
@@ -2500,6 +2529,9 @@
       <c r="I8">
         <v>3</v>
       </c>
+      <c r="J8" s="1" t="s">
+        <v>421</v>
+      </c>
       <c r="N8">
         <v>5</v>
       </c>
@@ -8356,12 +8388,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M122">
-    <sortState ref="A2:M125">
+  <autoFilter ref="A1:M122" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M125">
       <sortCondition ref="C1:C122"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:Q125">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q125">
     <sortCondition ref="C2:C125"/>
     <sortCondition ref="A2:A125"/>
   </sortState>

</xml_diff>

<commit_message>
Merged PR 339: V3.1.7 Beta 7
* Structure's bonds cannot be seen in ACME https://github.com/Chem4Word/Version3-1/issues/44
* ChEBI Search broken https://github.com/Chem4Word/Version3-1/issues/45

Related work items: #703
</commit_message>
<xml_diff>
--- a/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
+++ b/src/Chemistry/Chem4Word.Model2/Resources/PeriodicTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clyde\source\repos\Version3-1\src\Chemistry\Chem4Word.Model2\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE8FD7B-C9BB-45A3-8518-99E6548D1B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F857CCC-0EA9-4ABF-B1B7-FAA4C6288DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1815" yWindow="1290" windowWidth="24870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="422">
   <si>
     <t>Symbol</t>
   </si>
@@ -1305,7 +1305,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1443,6 +1443,12 @@
     <font>
       <sz val="10"/>
       <name val="Helv"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2143,10 +2149,10 @@
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="J125" sqref="J125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7029,6 +7035,9 @@
       <c r="I96">
         <v>-227.02780000000001</v>
       </c>
+      <c r="J96" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L96">
         <v>3</v>
       </c>
@@ -7488,6 +7497,9 @@
       <c r="I105">
         <v>-251.0796</v>
       </c>
+      <c r="J105" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L105">
         <v>3</v>
       </c>
@@ -7536,6 +7548,9 @@
       <c r="I106">
         <v>-252.083</v>
       </c>
+      <c r="J106" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L106">
         <v>3</v>
       </c>
@@ -7584,6 +7599,9 @@
       <c r="I107">
         <v>-257.0951</v>
       </c>
+      <c r="J107" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L107">
         <v>3</v>
       </c>
@@ -7683,6 +7701,9 @@
       <c r="I109">
         <v>-259.10109999999997</v>
       </c>
+      <c r="J109" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L109">
         <v>3</v>
       </c>
@@ -7782,6 +7803,9 @@
       <c r="I111">
         <v>-261.10890000000001</v>
       </c>
+      <c r="J111" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L111">
         <v>4</v>
       </c>
@@ -7830,6 +7854,9 @@
       <c r="I112">
         <v>-262.11439999999999</v>
       </c>
+      <c r="J112" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L112">
         <v>5</v>
       </c>
@@ -7878,6 +7905,9 @@
       <c r="I113">
         <v>-263.11860000000001</v>
       </c>
+      <c r="J113" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L113">
         <v>6</v>
       </c>
@@ -7926,6 +7956,9 @@
       <c r="I114">
         <v>-262.12310000000002</v>
       </c>
+      <c r="J114" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L114">
         <v>7</v>
       </c>
@@ -7971,6 +8004,9 @@
       <c r="I115">
         <v>-265.13060000000002</v>
       </c>
+      <c r="J115" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L115">
         <v>8</v>
       </c>
@@ -8016,6 +8052,9 @@
       <c r="I116">
         <v>-266.13780000000003</v>
       </c>
+      <c r="J116" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L116">
         <v>9</v>
       </c>
@@ -8058,6 +8097,9 @@
       <c r="I117">
         <v>-268</v>
       </c>
+      <c r="J117" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="L117">
         <v>10</v>
       </c>
@@ -8100,6 +8142,9 @@
       <c r="I118">
         <v>-269</v>
       </c>
+      <c r="J118" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N118">
         <v>6</v>
       </c>
@@ -8139,6 +8184,9 @@
       <c r="I119">
         <v>0</v>
       </c>
+      <c r="J119" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N119">
         <v>6</v>
       </c>
@@ -8178,6 +8226,9 @@
       <c r="I120">
         <v>0</v>
       </c>
+      <c r="J120" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N120">
         <v>6</v>
       </c>
@@ -8217,6 +8268,9 @@
       <c r="I121">
         <v>0</v>
       </c>
+      <c r="J121" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N121">
         <v>6</v>
       </c>
@@ -8256,6 +8310,9 @@
       <c r="I122">
         <v>0</v>
       </c>
+      <c r="J122" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N122">
         <v>6</v>
       </c>
@@ -8295,6 +8352,9 @@
       <c r="I123">
         <v>0</v>
       </c>
+      <c r="J123" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N123">
         <v>6</v>
       </c>
@@ -8334,6 +8394,9 @@
       <c r="I124">
         <v>0</v>
       </c>
+      <c r="J124" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="N124">
         <v>6</v>
       </c>
@@ -8372,6 +8435,9 @@
       </c>
       <c r="I125">
         <v>0</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>420</v>
       </c>
       <c r="N125">
         <v>6</v>
@@ -8397,6 +8463,7 @@
     <sortCondition ref="C2:C125"/>
     <sortCondition ref="A2:A125"/>
   </sortState>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>